<commit_message>
Add bai tap mang 2
</commit_message>
<xml_diff>
--- a/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
+++ b/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
@@ -496,10 +496,45 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -508,9 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -521,41 +553,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +771,8 @@
   <dimension ref="A1:J557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
+      <pane ySplit="2" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E120" sqref="E120:F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -790,50 +790,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="59" t="s">
+      <c r="B1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1"/>
-      <c r="J1" s="57"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="58"/>
+      <c r="J2" s="50"/>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46">
-        <v>1</v>
-      </c>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="53">
+        <v>1</v>
+      </c>
+      <c r="B3" s="63" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="36">
@@ -854,8 +854,8 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="49"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="36">
         <v>43986</v>
       </c>
@@ -874,8 +874,8 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="36">
         <v>43987</v>
       </c>
@@ -894,8 +894,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="36">
         <v>43988</v>
       </c>
@@ -914,8 +914,8 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="36">
         <v>43989</v>
       </c>
@@ -934,8 +934,8 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="36">
         <v>43990</v>
       </c>
@@ -954,8 +954,8 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="36">
         <v>43992</v>
       </c>
@@ -974,8 +974,8 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="36">
         <v>43994</v>
       </c>
@@ -994,8 +994,8 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="36">
         <v>43996</v>
       </c>
@@ -1014,8 +1014,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="36">
         <v>43998</v>
       </c>
@@ -1034,8 +1034,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="64"/>
       <c r="C13" s="36">
         <v>44000</v>
       </c>
@@ -1054,8 +1054,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="36">
         <v>44002</v>
       </c>
@@ -1074,8 +1074,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="36">
         <v>44004</v>
       </c>
@@ -1094,8 +1094,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="36">
         <v>44006</v>
       </c>
@@ -1114,10 +1114,10 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51">
-        <v>2</v>
-      </c>
-      <c r="B17" s="52" t="s">
+      <c r="A17" s="52">
+        <v>2</v>
+      </c>
+      <c r="B17" s="66" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="37">
@@ -1138,8 +1138,8 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="53"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="37">
         <v>43986</v>
       </c>
@@ -1158,8 +1158,8 @@
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="37">
         <v>43987</v>
       </c>
@@ -1178,8 +1178,8 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="37">
         <v>43988</v>
       </c>
@@ -1198,8 +1198,8 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="37">
         <v>43989</v>
       </c>
@@ -1218,8 +1218,8 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="37">
         <v>43990</v>
       </c>
@@ -1238,8 +1238,8 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="37">
         <v>43992</v>
       </c>
@@ -1258,8 +1258,8 @@
       <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="37">
         <v>43994</v>
       </c>
@@ -1278,8 +1278,8 @@
       <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="37">
         <v>43996</v>
       </c>
@@ -1298,8 +1298,8 @@
       <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="37">
         <v>43998</v>
       </c>
@@ -1318,8 +1318,8 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="37">
         <v>44000</v>
       </c>
@@ -1338,8 +1338,8 @@
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="53"/>
+      <c r="A28" s="49"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="37">
         <v>44002</v>
       </c>
@@ -1358,8 +1358,8 @@
       <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="67"/>
       <c r="C29" s="37">
         <v>44004</v>
       </c>
@@ -1378,8 +1378,8 @@
       <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="37">
         <v>44006</v>
       </c>
@@ -1398,10 +1398,10 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46">
+      <c r="A31" s="53">
         <v>3</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="69" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="36">
@@ -1422,8 +1422,8 @@
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="49"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="36">
         <v>43986</v>
       </c>
@@ -1442,8 +1442,8 @@
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="49"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="36">
         <v>43987</v>
       </c>
@@ -1462,8 +1462,8 @@
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="64"/>
       <c r="C34" s="36">
         <v>43988</v>
       </c>
@@ -1482,8 +1482,8 @@
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="36">
         <v>43989</v>
       </c>
@@ -1502,8 +1502,8 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="49"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="36">
         <v>43990</v>
       </c>
@@ -1522,8 +1522,8 @@
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="36">
         <v>43992</v>
       </c>
@@ -1542,8 +1542,8 @@
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="49"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="36">
         <v>43994</v>
       </c>
@@ -1562,8 +1562,8 @@
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="36">
         <v>43996</v>
       </c>
@@ -1582,8 +1582,8 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="49"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="36">
         <v>43998</v>
       </c>
@@ -1602,8 +1602,8 @@
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="49"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="64"/>
       <c r="C41" s="36">
         <v>44000</v>
       </c>
@@ -1622,8 +1622,8 @@
       <c r="J41" s="10"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="64"/>
       <c r="C42" s="36">
         <v>44002</v>
       </c>
@@ -1642,8 +1642,8 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="64"/>
       <c r="C43" s="36">
         <v>44004</v>
       </c>
@@ -1662,8 +1662,8 @@
       <c r="J43" s="10"/>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="50"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="36">
         <v>44006</v>
       </c>
@@ -1682,10 +1682,10 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="51">
+      <c r="A45" s="52">
         <v>4</v>
       </c>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="37">
@@ -1706,8 +1706,8 @@
       <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="47"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="37">
         <v>43986</v>
       </c>
@@ -1726,8 +1726,8 @@
       <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
+      <c r="A47" s="49"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="37">
         <v>43987</v>
       </c>
@@ -1746,8 +1746,8 @@
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
-      <c r="B48" s="47"/>
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
       <c r="C48" s="37">
         <v>43988</v>
       </c>
@@ -1766,8 +1766,8 @@
       <c r="J48" s="20"/>
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="47"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
       <c r="C49" s="37">
         <v>43989</v>
       </c>
@@ -1786,8 +1786,8 @@
       <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="37">
         <v>43990</v>
       </c>
@@ -1806,8 +1806,8 @@
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="37">
         <v>43992</v>
       </c>
@@ -1826,8 +1826,8 @@
       <c r="J51" s="22"/>
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="49"/>
+      <c r="B52" s="49"/>
       <c r="C52" s="37">
         <v>43994</v>
       </c>
@@ -1846,8 +1846,8 @@
       <c r="J52" s="22"/>
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="37">
         <v>43996</v>
       </c>
@@ -1866,8 +1866,8 @@
       <c r="J53" s="22"/>
     </row>
     <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="49"/>
       <c r="C54" s="37">
         <v>43998</v>
       </c>
@@ -1886,8 +1886,8 @@
       <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="47"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="49"/>
       <c r="C55" s="37">
         <v>44000</v>
       </c>
@@ -1906,8 +1906,8 @@
       <c r="J55" s="22"/>
     </row>
     <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="47"/>
-      <c r="B56" s="47"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="37">
         <v>44002</v>
       </c>
@@ -1926,8 +1926,8 @@
       <c r="J56" s="22"/>
     </row>
     <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
-      <c r="B57" s="47"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
       <c r="C57" s="37">
         <v>44004</v>
       </c>
@@ -1946,8 +1946,8 @@
       <c r="J57" s="22"/>
     </row>
     <row r="58" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="47"/>
-      <c r="B58" s="58"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="50"/>
       <c r="C58" s="37">
         <v>44006</v>
       </c>
@@ -1966,10 +1966,10 @@
       <c r="J58" s="22"/>
     </row>
     <row r="59" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="46">
+      <c r="A59" s="53">
         <v>5</v>
       </c>
-      <c r="B59" s="64" t="s">
+      <c r="B59" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C59" s="36">
@@ -1990,8 +1990,8 @@
       <c r="J59" s="6"/>
     </row>
     <row r="60" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="47"/>
-      <c r="B60" s="47"/>
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
       <c r="C60" s="36">
         <v>43986</v>
       </c>
@@ -2010,8 +2010,8 @@
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="47"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="49"/>
       <c r="C61" s="36">
         <v>43987</v>
       </c>
@@ -2030,8 +2030,8 @@
       <c r="J61" s="6"/>
     </row>
     <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="47"/>
+      <c r="A62" s="49"/>
+      <c r="B62" s="49"/>
       <c r="C62" s="36">
         <v>43988</v>
       </c>
@@ -2050,8 +2050,8 @@
       <c r="J62" s="6"/>
     </row>
     <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
-      <c r="B63" s="47"/>
+      <c r="A63" s="49"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="36">
         <v>43989</v>
       </c>
@@ -2070,8 +2070,8 @@
       <c r="J63" s="6"/>
     </row>
     <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
-      <c r="B64" s="47"/>
+      <c r="A64" s="49"/>
+      <c r="B64" s="49"/>
       <c r="C64" s="36">
         <v>43990</v>
       </c>
@@ -2090,8 +2090,8 @@
       <c r="J64" s="6"/>
     </row>
     <row r="65" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="47"/>
-      <c r="B65" s="47"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="49"/>
       <c r="C65" s="36">
         <v>43992</v>
       </c>
@@ -2110,8 +2110,8 @@
       <c r="J65" s="6"/>
     </row>
     <row r="66" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="47"/>
-      <c r="B66" s="47"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="49"/>
       <c r="C66" s="36">
         <v>43994</v>
       </c>
@@ -2130,8 +2130,8 @@
       <c r="J66" s="6"/>
     </row>
     <row r="67" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="47"/>
-      <c r="B67" s="47"/>
+      <c r="A67" s="49"/>
+      <c r="B67" s="49"/>
       <c r="C67" s="36">
         <v>43996</v>
       </c>
@@ -2150,8 +2150,8 @@
       <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="47"/>
-      <c r="B68" s="47"/>
+      <c r="A68" s="49"/>
+      <c r="B68" s="49"/>
       <c r="C68" s="36">
         <v>43998</v>
       </c>
@@ -2170,8 +2170,8 @@
       <c r="J68" s="6"/>
     </row>
     <row r="69" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
-      <c r="B69" s="47"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="49"/>
       <c r="C69" s="36">
         <v>44000</v>
       </c>
@@ -2190,8 +2190,8 @@
       <c r="J69" s="6"/>
     </row>
     <row r="70" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
-      <c r="B70" s="47"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="49"/>
       <c r="C70" s="36">
         <v>44002</v>
       </c>
@@ -2210,8 +2210,8 @@
       <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="47"/>
-      <c r="B71" s="47"/>
+      <c r="A71" s="49"/>
+      <c r="B71" s="49"/>
       <c r="C71" s="36">
         <v>44004</v>
       </c>
@@ -2230,8 +2230,8 @@
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="47"/>
-      <c r="B72" s="58"/>
+      <c r="A72" s="49"/>
+      <c r="B72" s="50"/>
       <c r="C72" s="36">
         <v>44006</v>
       </c>
@@ -2250,10 +2250,10 @@
       <c r="J72" s="6"/>
     </row>
     <row r="73" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="51">
+      <c r="A73" s="52">
         <v>6</v>
       </c>
-      <c r="B73" s="63" t="s">
+      <c r="B73" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="37">
@@ -2274,8 +2274,8 @@
       <c r="J73" s="20"/>
     </row>
     <row r="74" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
-      <c r="B74" s="47"/>
+      <c r="A74" s="49"/>
+      <c r="B74" s="49"/>
       <c r="C74" s="37">
         <v>43986</v>
       </c>
@@ -2294,8 +2294,8 @@
       <c r="J74" s="20"/>
     </row>
     <row r="75" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="47"/>
-      <c r="B75" s="47"/>
+      <c r="A75" s="49"/>
+      <c r="B75" s="49"/>
       <c r="C75" s="37">
         <v>43987</v>
       </c>
@@ -2314,8 +2314,8 @@
       <c r="J75" s="20"/>
     </row>
     <row r="76" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="47"/>
-      <c r="B76" s="47"/>
+      <c r="A76" s="49"/>
+      <c r="B76" s="49"/>
       <c r="C76" s="37">
         <v>43988</v>
       </c>
@@ -2334,8 +2334,8 @@
       <c r="J76" s="20"/>
     </row>
     <row r="77" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="47"/>
-      <c r="B77" s="47"/>
+      <c r="A77" s="49"/>
+      <c r="B77" s="49"/>
       <c r="C77" s="37">
         <v>43989</v>
       </c>
@@ -2354,8 +2354,8 @@
       <c r="J77" s="20"/>
     </row>
     <row r="78" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="47"/>
-      <c r="B78" s="47"/>
+      <c r="A78" s="49"/>
+      <c r="B78" s="49"/>
       <c r="C78" s="37">
         <v>43990</v>
       </c>
@@ -2374,8 +2374,8 @@
       <c r="J78" s="20"/>
     </row>
     <row r="79" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="47"/>
+      <c r="A79" s="49"/>
+      <c r="B79" s="49"/>
       <c r="C79" s="37">
         <v>43992</v>
       </c>
@@ -2394,8 +2394,8 @@
       <c r="J79" s="22"/>
     </row>
     <row r="80" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="47"/>
+      <c r="A80" s="49"/>
+      <c r="B80" s="49"/>
       <c r="C80" s="37">
         <v>43994</v>
       </c>
@@ -2414,8 +2414,8 @@
       <c r="J80" s="22"/>
     </row>
     <row r="81" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="47"/>
+      <c r="A81" s="49"/>
+      <c r="B81" s="49"/>
       <c r="C81" s="37">
         <v>43996</v>
       </c>
@@ -2434,8 +2434,8 @@
       <c r="J81" s="22"/>
     </row>
     <row r="82" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="47"/>
-      <c r="B82" s="47"/>
+      <c r="A82" s="49"/>
+      <c r="B82" s="49"/>
       <c r="C82" s="37">
         <v>43998</v>
       </c>
@@ -2454,8 +2454,8 @@
       <c r="J82" s="22"/>
     </row>
     <row r="83" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="47"/>
-      <c r="B83" s="47"/>
+      <c r="A83" s="49"/>
+      <c r="B83" s="49"/>
       <c r="C83" s="37">
         <v>44000</v>
       </c>
@@ -2474,8 +2474,8 @@
       <c r="J83" s="22"/>
     </row>
     <row r="84" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
-      <c r="B84" s="47"/>
+      <c r="A84" s="49"/>
+      <c r="B84" s="49"/>
       <c r="C84" s="37">
         <v>44002</v>
       </c>
@@ -2494,8 +2494,8 @@
       <c r="J84" s="22"/>
     </row>
     <row r="85" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="47"/>
-      <c r="B85" s="47"/>
+      <c r="A85" s="49"/>
+      <c r="B85" s="49"/>
       <c r="C85" s="37">
         <v>44004</v>
       </c>
@@ -2514,8 +2514,8 @@
       <c r="J85" s="22"/>
     </row>
     <row r="86" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="47"/>
-      <c r="B86" s="58"/>
+      <c r="A86" s="49"/>
+      <c r="B86" s="50"/>
       <c r="C86" s="37">
         <v>44006</v>
       </c>
@@ -2534,10 +2534,10 @@
       <c r="J86" s="22"/>
     </row>
     <row r="87" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="46">
+      <c r="A87" s="53">
         <v>7</v>
       </c>
-      <c r="B87" s="64" t="s">
+      <c r="B87" s="51" t="s">
         <v>18</v>
       </c>
       <c r="C87" s="36">
@@ -2558,8 +2558,8 @@
       <c r="J87" s="6"/>
     </row>
     <row r="88" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="47"/>
-      <c r="B88" s="47"/>
+      <c r="A88" s="49"/>
+      <c r="B88" s="49"/>
       <c r="C88" s="36">
         <v>43986</v>
       </c>
@@ -2578,8 +2578,8 @@
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="47"/>
-      <c r="B89" s="47"/>
+      <c r="A89" s="49"/>
+      <c r="B89" s="49"/>
       <c r="C89" s="36">
         <v>43987</v>
       </c>
@@ -2598,8 +2598,8 @@
       <c r="J89" s="6"/>
     </row>
     <row r="90" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="47"/>
-      <c r="B90" s="47"/>
+      <c r="A90" s="49"/>
+      <c r="B90" s="49"/>
       <c r="C90" s="36">
         <v>43988</v>
       </c>
@@ -2618,8 +2618,8 @@
       <c r="J90" s="6"/>
     </row>
     <row r="91" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="47"/>
-      <c r="B91" s="47"/>
+      <c r="A91" s="49"/>
+      <c r="B91" s="49"/>
       <c r="C91" s="36">
         <v>43989</v>
       </c>
@@ -2638,8 +2638,8 @@
       <c r="J91" s="6"/>
     </row>
     <row r="92" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="47"/>
-      <c r="B92" s="47"/>
+      <c r="A92" s="49"/>
+      <c r="B92" s="49"/>
       <c r="C92" s="36">
         <v>43990</v>
       </c>
@@ -2658,8 +2658,8 @@
       <c r="J92" s="6"/>
     </row>
     <row r="93" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
-      <c r="B93" s="47"/>
+      <c r="A93" s="49"/>
+      <c r="B93" s="49"/>
       <c r="C93" s="36">
         <v>43992</v>
       </c>
@@ -2678,8 +2678,8 @@
       <c r="J93" s="10"/>
     </row>
     <row r="94" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="47"/>
-      <c r="B94" s="47"/>
+      <c r="A94" s="49"/>
+      <c r="B94" s="49"/>
       <c r="C94" s="36">
         <v>43994</v>
       </c>
@@ -2698,8 +2698,8 @@
       <c r="J94" s="10"/>
     </row>
     <row r="95" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="47"/>
-      <c r="B95" s="47"/>
+      <c r="A95" s="49"/>
+      <c r="B95" s="49"/>
       <c r="C95" s="36">
         <v>43996</v>
       </c>
@@ -2718,8 +2718,8 @@
       <c r="J95" s="10"/>
     </row>
     <row r="96" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="47"/>
-      <c r="B96" s="47"/>
+      <c r="A96" s="49"/>
+      <c r="B96" s="49"/>
       <c r="C96" s="36">
         <v>43998</v>
       </c>
@@ -2738,8 +2738,8 @@
       <c r="J96" s="10"/>
     </row>
     <row r="97" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="47"/>
-      <c r="B97" s="47"/>
+      <c r="A97" s="49"/>
+      <c r="B97" s="49"/>
       <c r="C97" s="36">
         <v>44000</v>
       </c>
@@ -2758,8 +2758,8 @@
       <c r="J97" s="10"/>
     </row>
     <row r="98" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="47"/>
-      <c r="B98" s="47"/>
+      <c r="A98" s="49"/>
+      <c r="B98" s="49"/>
       <c r="C98" s="36">
         <v>44002</v>
       </c>
@@ -2778,8 +2778,8 @@
       <c r="J98" s="10"/>
     </row>
     <row r="99" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="47"/>
-      <c r="B99" s="47"/>
+      <c r="A99" s="49"/>
+      <c r="B99" s="49"/>
       <c r="C99" s="36">
         <v>44004</v>
       </c>
@@ -2798,8 +2798,8 @@
       <c r="J99" s="10"/>
     </row>
     <row r="100" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
-      <c r="B100" s="58"/>
+      <c r="A100" s="49"/>
+      <c r="B100" s="50"/>
       <c r="C100" s="36">
         <v>44006</v>
       </c>
@@ -2818,10 +2818,10 @@
       <c r="J100" s="10"/>
     </row>
     <row r="101" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="51">
+      <c r="A101" s="52">
         <v>8</v>
       </c>
-      <c r="B101" s="63" t="s">
+      <c r="B101" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C101" s="37">
@@ -2842,8 +2842,8 @@
       <c r="J101" s="20"/>
     </row>
     <row r="102" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
-      <c r="B102" s="47"/>
+      <c r="A102" s="49"/>
+      <c r="B102" s="49"/>
       <c r="C102" s="37">
         <v>43986</v>
       </c>
@@ -2862,8 +2862,8 @@
       <c r="J102" s="20"/>
     </row>
     <row r="103" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="47"/>
-      <c r="B103" s="47"/>
+      <c r="A103" s="49"/>
+      <c r="B103" s="49"/>
       <c r="C103" s="37">
         <v>43987</v>
       </c>
@@ -2882,8 +2882,8 @@
       <c r="J103" s="20"/>
     </row>
     <row r="104" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="47"/>
-      <c r="B104" s="47"/>
+      <c r="A104" s="49"/>
+      <c r="B104" s="49"/>
       <c r="C104" s="37">
         <v>43988</v>
       </c>
@@ -2902,8 +2902,8 @@
       <c r="J104" s="20"/>
     </row>
     <row r="105" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="47"/>
-      <c r="B105" s="47"/>
+      <c r="A105" s="49"/>
+      <c r="B105" s="49"/>
       <c r="C105" s="37">
         <v>43989</v>
       </c>
@@ -2922,8 +2922,8 @@
       <c r="J105" s="20"/>
     </row>
     <row r="106" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="47"/>
-      <c r="B106" s="47"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="49"/>
       <c r="C106" s="37">
         <v>43990</v>
       </c>
@@ -2942,8 +2942,8 @@
       <c r="J106" s="20"/>
     </row>
     <row r="107" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="47"/>
-      <c r="B107" s="47"/>
+      <c r="A107" s="49"/>
+      <c r="B107" s="49"/>
       <c r="C107" s="37">
         <v>43992</v>
       </c>
@@ -2962,8 +2962,8 @@
       <c r="J107" s="22"/>
     </row>
     <row r="108" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="47"/>
-      <c r="B108" s="47"/>
+      <c r="A108" s="49"/>
+      <c r="B108" s="49"/>
       <c r="C108" s="37">
         <v>43994</v>
       </c>
@@ -2982,8 +2982,8 @@
       <c r="J108" s="22"/>
     </row>
     <row r="109" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="47"/>
-      <c r="B109" s="47"/>
+      <c r="A109" s="49"/>
+      <c r="B109" s="49"/>
       <c r="C109" s="37">
         <v>43996</v>
       </c>
@@ -3002,8 +3002,8 @@
       <c r="J109" s="22"/>
     </row>
     <row r="110" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="47"/>
-      <c r="B110" s="47"/>
+      <c r="A110" s="49"/>
+      <c r="B110" s="49"/>
       <c r="C110" s="37">
         <v>43998</v>
       </c>
@@ -3022,8 +3022,8 @@
       <c r="J110" s="22"/>
     </row>
     <row r="111" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="47"/>
-      <c r="B111" s="47"/>
+      <c r="A111" s="49"/>
+      <c r="B111" s="49"/>
       <c r="C111" s="37">
         <v>44000</v>
       </c>
@@ -3042,8 +3042,8 @@
       <c r="J111" s="22"/>
     </row>
     <row r="112" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="47"/>
-      <c r="B112" s="47"/>
+      <c r="A112" s="49"/>
+      <c r="B112" s="49"/>
       <c r="C112" s="37">
         <v>44002</v>
       </c>
@@ -3062,8 +3062,8 @@
       <c r="J112" s="22"/>
     </row>
     <row r="113" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="47"/>
-      <c r="B113" s="47"/>
+      <c r="A113" s="49"/>
+      <c r="B113" s="49"/>
       <c r="C113" s="37">
         <v>44004</v>
       </c>
@@ -3082,8 +3082,8 @@
       <c r="J113" s="22"/>
     </row>
     <row r="114" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="47"/>
-      <c r="B114" s="58"/>
+      <c r="A114" s="49"/>
+      <c r="B114" s="50"/>
       <c r="C114" s="37">
         <v>44006</v>
       </c>
@@ -3102,10 +3102,10 @@
       <c r="J114" s="22"/>
     </row>
     <row r="115" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="46">
+      <c r="A115" s="53">
         <v>9</v>
       </c>
-      <c r="B115" s="65" t="s">
+      <c r="B115" s="54" t="s">
         <v>20</v>
       </c>
       <c r="C115" s="36">
@@ -3126,8 +3126,8 @@
       <c r="J115" s="6"/>
     </row>
     <row r="116" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="47"/>
-      <c r="B116" s="66"/>
+      <c r="A116" s="49"/>
+      <c r="B116" s="55"/>
       <c r="C116" s="36">
         <v>43986</v>
       </c>
@@ -3146,18 +3146,18 @@
       <c r="J116" s="6"/>
     </row>
     <row r="117" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="47"/>
-      <c r="B117" s="66"/>
+      <c r="A117" s="49"/>
+      <c r="B117" s="55"/>
       <c r="C117" s="36">
         <v>43987</v>
       </c>
       <c r="D117" s="36">
         <v>43987</v>
       </c>
-      <c r="E117" s="69">
-        <v>2</v>
-      </c>
-      <c r="F117" s="68">
+      <c r="E117" s="47">
+        <v>2</v>
+      </c>
+      <c r="F117" s="46">
         <v>1</v>
       </c>
       <c r="G117" s="41"/>
@@ -3166,18 +3166,18 @@
       <c r="J117" s="6"/>
     </row>
     <row r="118" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="47"/>
-      <c r="B118" s="66"/>
+      <c r="A118" s="49"/>
+      <c r="B118" s="55"/>
       <c r="C118" s="36">
         <v>43988</v>
       </c>
       <c r="D118" s="36">
         <v>43988</v>
       </c>
-      <c r="E118" s="68">
-        <v>2</v>
-      </c>
-      <c r="F118" s="68">
+      <c r="E118" s="46">
+        <v>2</v>
+      </c>
+      <c r="F118" s="46">
         <v>2</v>
       </c>
       <c r="G118" s="41"/>
@@ -3186,18 +3186,18 @@
       <c r="J118" s="6"/>
     </row>
     <row r="119" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="47"/>
-      <c r="B119" s="66"/>
+      <c r="A119" s="49"/>
+      <c r="B119" s="55"/>
       <c r="C119" s="36">
         <v>43989</v>
       </c>
       <c r="D119" s="36">
         <v>43989</v>
       </c>
-      <c r="E119" s="68">
-        <v>2</v>
-      </c>
-      <c r="F119" s="68">
+      <c r="E119" s="46">
+        <v>2</v>
+      </c>
+      <c r="F119" s="46">
         <v>3</v>
       </c>
       <c r="G119" s="41"/>
@@ -3206,18 +3206,18 @@
       <c r="J119" s="6"/>
     </row>
     <row r="120" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
-      <c r="B120" s="66"/>
+      <c r="A120" s="49"/>
+      <c r="B120" s="55"/>
       <c r="C120" s="36">
         <v>43990</v>
       </c>
       <c r="D120" s="36">
         <v>43991</v>
       </c>
-      <c r="E120" s="3">
+      <c r="E120" s="46">
         <v>3</v>
       </c>
-      <c r="F120" s="3">
+      <c r="F120" s="46">
         <v>1</v>
       </c>
       <c r="G120" s="41"/>
@@ -3226,18 +3226,18 @@
       <c r="J120" s="6"/>
     </row>
     <row r="121" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="47"/>
-      <c r="B121" s="66"/>
+      <c r="A121" s="49"/>
+      <c r="B121" s="55"/>
       <c r="C121" s="36">
         <v>43992</v>
       </c>
       <c r="D121" s="36">
         <v>43993</v>
       </c>
-      <c r="E121" s="3">
+      <c r="E121" s="46">
         <v>3</v>
       </c>
-      <c r="F121" s="8">
+      <c r="F121" s="46">
         <v>2</v>
       </c>
       <c r="G121" s="41"/>
@@ -3246,8 +3246,8 @@
       <c r="J121" s="10"/>
     </row>
     <row r="122" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="47"/>
-      <c r="B122" s="66"/>
+      <c r="A122" s="49"/>
+      <c r="B122" s="55"/>
       <c r="C122" s="36">
         <v>43994</v>
       </c>
@@ -3266,8 +3266,8 @@
       <c r="J122" s="10"/>
     </row>
     <row r="123" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="47"/>
-      <c r="B123" s="66"/>
+      <c r="A123" s="49"/>
+      <c r="B123" s="55"/>
       <c r="C123" s="36">
         <v>43996</v>
       </c>
@@ -3286,8 +3286,8 @@
       <c r="J123" s="10"/>
     </row>
     <row r="124" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="47"/>
-      <c r="B124" s="66"/>
+      <c r="A124" s="49"/>
+      <c r="B124" s="55"/>
       <c r="C124" s="36">
         <v>43998</v>
       </c>
@@ -3306,8 +3306,8 @@
       <c r="J124" s="10"/>
     </row>
     <row r="125" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="47"/>
-      <c r="B125" s="66"/>
+      <c r="A125" s="49"/>
+      <c r="B125" s="55"/>
       <c r="C125" s="36">
         <v>44000</v>
       </c>
@@ -3326,8 +3326,8 @@
       <c r="J125" s="10"/>
     </row>
     <row r="126" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="47"/>
-      <c r="B126" s="66"/>
+      <c r="A126" s="49"/>
+      <c r="B126" s="55"/>
       <c r="C126" s="36">
         <v>44002</v>
       </c>
@@ -3346,8 +3346,8 @@
       <c r="J126" s="10"/>
     </row>
     <row r="127" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="47"/>
-      <c r="B127" s="66"/>
+      <c r="A127" s="49"/>
+      <c r="B127" s="55"/>
       <c r="C127" s="36">
         <v>44004</v>
       </c>
@@ -3366,8 +3366,8 @@
       <c r="J127" s="10"/>
     </row>
     <row r="128" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="47"/>
-      <c r="B128" s="67"/>
+      <c r="A128" s="49"/>
+      <c r="B128" s="56"/>
       <c r="C128" s="36">
         <v>44006</v>
       </c>
@@ -3386,10 +3386,10 @@
       <c r="J128" s="10"/>
     </row>
     <row r="129" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="51">
+      <c r="A129" s="52">
         <v>10</v>
       </c>
-      <c r="B129" s="63" t="s">
+      <c r="B129" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C129" s="37">
@@ -3410,8 +3410,8 @@
       <c r="J129" s="20"/>
     </row>
     <row r="130" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="47"/>
-      <c r="B130" s="47"/>
+      <c r="A130" s="49"/>
+      <c r="B130" s="49"/>
       <c r="C130" s="37">
         <v>43986</v>
       </c>
@@ -3430,8 +3430,8 @@
       <c r="J130" s="20"/>
     </row>
     <row r="131" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="47"/>
-      <c r="B131" s="47"/>
+      <c r="A131" s="49"/>
+      <c r="B131" s="49"/>
       <c r="C131" s="37">
         <v>43987</v>
       </c>
@@ -3450,8 +3450,8 @@
       <c r="J131" s="20"/>
     </row>
     <row r="132" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="47"/>
-      <c r="B132" s="47"/>
+      <c r="A132" s="49"/>
+      <c r="B132" s="49"/>
       <c r="C132" s="37">
         <v>43988</v>
       </c>
@@ -3470,8 +3470,8 @@
       <c r="J132" s="20"/>
     </row>
     <row r="133" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="47"/>
-      <c r="B133" s="47"/>
+      <c r="A133" s="49"/>
+      <c r="B133" s="49"/>
       <c r="C133" s="37">
         <v>43989</v>
       </c>
@@ -3490,8 +3490,8 @@
       <c r="J133" s="20"/>
     </row>
     <row r="134" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="47"/>
-      <c r="B134" s="47"/>
+      <c r="A134" s="49"/>
+      <c r="B134" s="49"/>
       <c r="C134" s="37">
         <v>43990</v>
       </c>
@@ -3510,8 +3510,8 @@
       <c r="J134" s="20"/>
     </row>
     <row r="135" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="47"/>
-      <c r="B135" s="47"/>
+      <c r="A135" s="49"/>
+      <c r="B135" s="49"/>
       <c r="C135" s="37">
         <v>43992</v>
       </c>
@@ -3530,8 +3530,8 @@
       <c r="J135" s="22"/>
     </row>
     <row r="136" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="47"/>
-      <c r="B136" s="47"/>
+      <c r="A136" s="49"/>
+      <c r="B136" s="49"/>
       <c r="C136" s="37">
         <v>43994</v>
       </c>
@@ -3550,8 +3550,8 @@
       <c r="J136" s="22"/>
     </row>
     <row r="137" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="47"/>
-      <c r="B137" s="47"/>
+      <c r="A137" s="49"/>
+      <c r="B137" s="49"/>
       <c r="C137" s="37">
         <v>43996</v>
       </c>
@@ -3570,8 +3570,8 @@
       <c r="J137" s="22"/>
     </row>
     <row r="138" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="47"/>
-      <c r="B138" s="47"/>
+      <c r="A138" s="49"/>
+      <c r="B138" s="49"/>
       <c r="C138" s="37">
         <v>43998</v>
       </c>
@@ -3590,8 +3590,8 @@
       <c r="J138" s="22"/>
     </row>
     <row r="139" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="47"/>
-      <c r="B139" s="47"/>
+      <c r="A139" s="49"/>
+      <c r="B139" s="49"/>
       <c r="C139" s="37">
         <v>44000</v>
       </c>
@@ -3610,8 +3610,8 @@
       <c r="J139" s="22"/>
     </row>
     <row r="140" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="47"/>
-      <c r="B140" s="47"/>
+      <c r="A140" s="49"/>
+      <c r="B140" s="49"/>
       <c r="C140" s="37">
         <v>44002</v>
       </c>
@@ -3630,8 +3630,8 @@
       <c r="J140" s="22"/>
     </row>
     <row r="141" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="47"/>
-      <c r="B141" s="47"/>
+      <c r="A141" s="49"/>
+      <c r="B141" s="49"/>
       <c r="C141" s="37">
         <v>44004</v>
       </c>
@@ -3650,8 +3650,8 @@
       <c r="J141" s="22"/>
     </row>
     <row r="142" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="47"/>
-      <c r="B142" s="58"/>
+      <c r="A142" s="49"/>
+      <c r="B142" s="50"/>
       <c r="C142" s="37">
         <v>44006</v>
       </c>
@@ -3670,10 +3670,10 @@
       <c r="J142" s="22"/>
     </row>
     <row r="143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="46">
+      <c r="A143" s="53">
         <v>11</v>
       </c>
-      <c r="B143" s="64" t="s">
+      <c r="B143" s="51" t="s">
         <v>22</v>
       </c>
       <c r="C143" s="36">
@@ -3693,8 +3693,8 @@
       <c r="I143" s="5"/>
     </row>
     <row r="144" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="47"/>
-      <c r="B144" s="47"/>
+      <c r="A144" s="49"/>
+      <c r="B144" s="49"/>
       <c r="C144" s="36">
         <v>43986</v>
       </c>
@@ -3712,8 +3712,8 @@
       <c r="I144" s="7"/>
     </row>
     <row r="145" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="47"/>
-      <c r="B145" s="47"/>
+      <c r="A145" s="49"/>
+      <c r="B145" s="49"/>
       <c r="C145" s="36">
         <v>43987</v>
       </c>
@@ -3731,8 +3731,8 @@
       <c r="I145" s="7"/>
     </row>
     <row r="146" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="47"/>
-      <c r="B146" s="47"/>
+      <c r="A146" s="49"/>
+      <c r="B146" s="49"/>
       <c r="C146" s="36">
         <v>43988</v>
       </c>
@@ -3750,8 +3750,8 @@
       <c r="I146" s="7"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="47"/>
-      <c r="B147" s="47"/>
+      <c r="A147" s="49"/>
+      <c r="B147" s="49"/>
       <c r="C147" s="36">
         <v>43989</v>
       </c>
@@ -3769,8 +3769,8 @@
       <c r="I147" s="7"/>
     </row>
     <row r="148" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="47"/>
-      <c r="B148" s="47"/>
+      <c r="A148" s="49"/>
+      <c r="B148" s="49"/>
       <c r="C148" s="36">
         <v>43990</v>
       </c>
@@ -3788,8 +3788,8 @@
       <c r="I148" s="7"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="47"/>
-      <c r="B149" s="47"/>
+      <c r="A149" s="49"/>
+      <c r="B149" s="49"/>
       <c r="C149" s="36">
         <v>43992</v>
       </c>
@@ -3807,8 +3807,8 @@
       <c r="I149" s="7"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="47"/>
-      <c r="B150" s="47"/>
+      <c r="A150" s="49"/>
+      <c r="B150" s="49"/>
       <c r="C150" s="36">
         <v>43994</v>
       </c>
@@ -3826,8 +3826,8 @@
       <c r="I150" s="7"/>
     </row>
     <row r="151" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="47"/>
-      <c r="B151" s="47"/>
+      <c r="A151" s="49"/>
+      <c r="B151" s="49"/>
       <c r="C151" s="36">
         <v>43996</v>
       </c>
@@ -3845,8 +3845,8 @@
       <c r="I151" s="7"/>
     </row>
     <row r="152" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="47"/>
-      <c r="B152" s="47"/>
+      <c r="A152" s="49"/>
+      <c r="B152" s="49"/>
       <c r="C152" s="36">
         <v>43998</v>
       </c>
@@ -3864,8 +3864,8 @@
       <c r="I152" s="12"/>
     </row>
     <row r="153" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="47"/>
-      <c r="B153" s="47"/>
+      <c r="A153" s="49"/>
+      <c r="B153" s="49"/>
       <c r="C153" s="36">
         <v>44000</v>
       </c>
@@ -3883,8 +3883,8 @@
       <c r="I153" s="12"/>
     </row>
     <row r="154" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="47"/>
-      <c r="B154" s="47"/>
+      <c r="A154" s="49"/>
+      <c r="B154" s="49"/>
       <c r="C154" s="36">
         <v>44002</v>
       </c>
@@ -3902,8 +3902,8 @@
       <c r="I154" s="12"/>
     </row>
     <row r="155" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="47"/>
-      <c r="B155" s="47"/>
+      <c r="A155" s="49"/>
+      <c r="B155" s="49"/>
       <c r="C155" s="36">
         <v>44004</v>
       </c>
@@ -3921,8 +3921,8 @@
       <c r="I155" s="12"/>
     </row>
     <row r="156" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="47"/>
-      <c r="B156" s="58"/>
+      <c r="A156" s="49"/>
+      <c r="B156" s="50"/>
       <c r="C156" s="36">
         <v>44006</v>
       </c>
@@ -3940,10 +3940,10 @@
       <c r="I156" s="9"/>
     </row>
     <row r="157" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="51">
+      <c r="A157" s="52">
         <v>12</v>
       </c>
-      <c r="B157" s="63" t="s">
+      <c r="B157" s="48" t="s">
         <v>11</v>
       </c>
       <c r="C157" s="37">
@@ -3964,8 +3964,8 @@
       <c r="J157" s="20"/>
     </row>
     <row r="158" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="47"/>
-      <c r="B158" s="47"/>
+      <c r="A158" s="49"/>
+      <c r="B158" s="49"/>
       <c r="C158" s="37">
         <v>43986</v>
       </c>
@@ -3984,8 +3984,8 @@
       <c r="J158" s="20"/>
     </row>
     <row r="159" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="47"/>
-      <c r="B159" s="47"/>
+      <c r="A159" s="49"/>
+      <c r="B159" s="49"/>
       <c r="C159" s="37">
         <v>43987</v>
       </c>
@@ -4004,8 +4004,8 @@
       <c r="J159" s="20"/>
     </row>
     <row r="160" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="47"/>
-      <c r="B160" s="47"/>
+      <c r="A160" s="49"/>
+      <c r="B160" s="49"/>
       <c r="C160" s="37">
         <v>43988</v>
       </c>
@@ -4024,8 +4024,8 @@
       <c r="J160" s="20"/>
     </row>
     <row r="161" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="47"/>
-      <c r="B161" s="47"/>
+      <c r="A161" s="49"/>
+      <c r="B161" s="49"/>
       <c r="C161" s="37">
         <v>43989</v>
       </c>
@@ -4044,8 +4044,8 @@
       <c r="J161" s="20"/>
     </row>
     <row r="162" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="47"/>
-      <c r="B162" s="47"/>
+      <c r="A162" s="49"/>
+      <c r="B162" s="49"/>
       <c r="C162" s="37">
         <v>43990</v>
       </c>
@@ -4064,8 +4064,8 @@
       <c r="J162" s="20"/>
     </row>
     <row r="163" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="47"/>
-      <c r="B163" s="47"/>
+      <c r="A163" s="49"/>
+      <c r="B163" s="49"/>
       <c r="C163" s="37">
         <v>43992</v>
       </c>
@@ -4084,8 +4084,8 @@
       <c r="J163" s="22"/>
     </row>
     <row r="164" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="47"/>
-      <c r="B164" s="47"/>
+      <c r="A164" s="49"/>
+      <c r="B164" s="49"/>
       <c r="C164" s="37">
         <v>43994</v>
       </c>
@@ -4104,8 +4104,8 @@
       <c r="J164" s="22"/>
     </row>
     <row r="165" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="47"/>
-      <c r="B165" s="47"/>
+      <c r="A165" s="49"/>
+      <c r="B165" s="49"/>
       <c r="C165" s="37">
         <v>43996</v>
       </c>
@@ -4124,8 +4124,8 @@
       <c r="J165" s="22"/>
     </row>
     <row r="166" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="47"/>
-      <c r="B166" s="47"/>
+      <c r="A166" s="49"/>
+      <c r="B166" s="49"/>
       <c r="C166" s="37">
         <v>43998</v>
       </c>
@@ -4144,8 +4144,8 @@
       <c r="J166" s="22"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="47"/>
-      <c r="B167" s="47"/>
+      <c r="A167" s="49"/>
+      <c r="B167" s="49"/>
       <c r="C167" s="37">
         <v>44000</v>
       </c>
@@ -4164,8 +4164,8 @@
       <c r="J167" s="22"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="47"/>
-      <c r="B168" s="47"/>
+      <c r="A168" s="49"/>
+      <c r="B168" s="49"/>
       <c r="C168" s="37">
         <v>44002</v>
       </c>
@@ -4184,8 +4184,8 @@
       <c r="J168" s="22"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="47"/>
-      <c r="B169" s="47"/>
+      <c r="A169" s="49"/>
+      <c r="B169" s="49"/>
       <c r="C169" s="37">
         <v>44004</v>
       </c>
@@ -4204,8 +4204,8 @@
       <c r="J169" s="22"/>
     </row>
     <row r="170" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="47"/>
-      <c r="B170" s="58"/>
+      <c r="A170" s="49"/>
+      <c r="B170" s="50"/>
       <c r="C170" s="37">
         <v>44006</v>
       </c>
@@ -4224,10 +4224,10 @@
       <c r="J170" s="22"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="46">
+      <c r="A171" s="53">
         <v>13</v>
       </c>
-      <c r="B171" s="64" t="s">
+      <c r="B171" s="51" t="s">
         <v>10</v>
       </c>
       <c r="C171" s="36">
@@ -4247,8 +4247,8 @@
       <c r="I171" s="5"/>
     </row>
     <row r="172" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="47"/>
-      <c r="B172" s="47"/>
+      <c r="A172" s="49"/>
+      <c r="B172" s="49"/>
       <c r="C172" s="36">
         <v>43986</v>
       </c>
@@ -4266,8 +4266,8 @@
       <c r="I172" s="7"/>
     </row>
     <row r="173" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="47"/>
-      <c r="B173" s="47"/>
+      <c r="A173" s="49"/>
+      <c r="B173" s="49"/>
       <c r="C173" s="36">
         <v>43987</v>
       </c>
@@ -4285,8 +4285,8 @@
       <c r="I173" s="7"/>
     </row>
     <row r="174" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="47"/>
-      <c r="B174" s="47"/>
+      <c r="A174" s="49"/>
+      <c r="B174" s="49"/>
       <c r="C174" s="36">
         <v>43988</v>
       </c>
@@ -4304,8 +4304,8 @@
       <c r="I174" s="7"/>
     </row>
     <row r="175" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="47"/>
-      <c r="B175" s="47"/>
+      <c r="A175" s="49"/>
+      <c r="B175" s="49"/>
       <c r="C175" s="36">
         <v>43989</v>
       </c>
@@ -4323,8 +4323,8 @@
       <c r="I175" s="7"/>
     </row>
     <row r="176" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="47"/>
-      <c r="B176" s="47"/>
+      <c r="A176" s="49"/>
+      <c r="B176" s="49"/>
       <c r="C176" s="36">
         <v>43990</v>
       </c>
@@ -4342,8 +4342,8 @@
       <c r="I176" s="7"/>
     </row>
     <row r="177" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="47"/>
-      <c r="B177" s="47"/>
+      <c r="A177" s="49"/>
+      <c r="B177" s="49"/>
       <c r="C177" s="36">
         <v>43992</v>
       </c>
@@ -4361,8 +4361,8 @@
       <c r="I177" s="7"/>
     </row>
     <row r="178" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="47"/>
-      <c r="B178" s="47"/>
+      <c r="A178" s="49"/>
+      <c r="B178" s="49"/>
       <c r="C178" s="36">
         <v>43994</v>
       </c>
@@ -4380,8 +4380,8 @@
       <c r="I178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="47"/>
-      <c r="B179" s="47"/>
+      <c r="A179" s="49"/>
+      <c r="B179" s="49"/>
       <c r="C179" s="36">
         <v>43996</v>
       </c>
@@ -4399,8 +4399,8 @@
       <c r="I179" s="9"/>
     </row>
     <row r="180" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="47"/>
-      <c r="B180" s="47"/>
+      <c r="A180" s="49"/>
+      <c r="B180" s="49"/>
       <c r="C180" s="36">
         <v>43998</v>
       </c>
@@ -4418,8 +4418,8 @@
       <c r="I180" s="12"/>
     </row>
     <row r="181" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="47"/>
-      <c r="B181" s="47"/>
+      <c r="A181" s="49"/>
+      <c r="B181" s="49"/>
       <c r="C181" s="36">
         <v>44000</v>
       </c>
@@ -4437,8 +4437,8 @@
       <c r="I181" s="12"/>
     </row>
     <row r="182" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="47"/>
-      <c r="B182" s="47"/>
+      <c r="A182" s="49"/>
+      <c r="B182" s="49"/>
       <c r="C182" s="36">
         <v>44002</v>
       </c>
@@ -4456,8 +4456,8 @@
       <c r="I182" s="12"/>
     </row>
     <row r="183" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="47"/>
-      <c r="B183" s="47"/>
+      <c r="A183" s="49"/>
+      <c r="B183" s="49"/>
       <c r="C183" s="36">
         <v>44004</v>
       </c>
@@ -4475,8 +4475,8 @@
       <c r="I183" s="12"/>
     </row>
     <row r="184" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="47"/>
-      <c r="B184" s="58"/>
+      <c r="A184" s="49"/>
+      <c r="B184" s="50"/>
       <c r="C184" s="36">
         <v>44006</v>
       </c>
@@ -4868,6 +4868,27 @@
     <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B17:B30"/>
+    <mergeCell ref="A31:A44"/>
+    <mergeCell ref="B31:B44"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B45:B58"/>
+    <mergeCell ref="A45:A58"/>
+    <mergeCell ref="A59:A72"/>
+    <mergeCell ref="A73:A86"/>
+    <mergeCell ref="B59:B72"/>
+    <mergeCell ref="B73:B86"/>
     <mergeCell ref="B157:B170"/>
     <mergeCell ref="B171:B184"/>
     <mergeCell ref="A157:A170"/>
@@ -4882,27 +4903,6 @@
     <mergeCell ref="B143:B156"/>
     <mergeCell ref="A143:A156"/>
     <mergeCell ref="B129:B142"/>
-    <mergeCell ref="B45:B58"/>
-    <mergeCell ref="A45:A58"/>
-    <mergeCell ref="A59:A72"/>
-    <mergeCell ref="A73:A86"/>
-    <mergeCell ref="B59:B72"/>
-    <mergeCell ref="B73:B86"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="B17:B30"/>
-    <mergeCell ref="A31:A44"/>
-    <mergeCell ref="B31:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add bai tap ham 2 continued...
</commit_message>
<xml_diff>
--- a/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
+++ b/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
@@ -397,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,43 +498,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -543,6 +510,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -556,6 +526,37 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,7 +773,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E120" sqref="E120:F121"/>
+      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -790,50 +791,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="60" t="s">
+      <c r="B1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="58" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1"/>
-      <c r="J1" s="59"/>
+      <c r="J1" s="60"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="50"/>
+      <c r="J2" s="61"/>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53">
-        <v>1</v>
-      </c>
-      <c r="B3" s="63" t="s">
+      <c r="A3" s="48">
+        <v>1</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="36">
@@ -855,7 +856,7 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49"/>
-      <c r="B4" s="64"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="36">
         <v>43986</v>
       </c>
@@ -875,7 +876,7 @@
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
-      <c r="B5" s="64"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="36">
         <v>43987</v>
       </c>
@@ -895,7 +896,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
-      <c r="B6" s="64"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="36">
         <v>43988</v>
       </c>
@@ -915,7 +916,7 @@
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
-      <c r="B7" s="64"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="36">
         <v>43989</v>
       </c>
@@ -935,7 +936,7 @@
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
-      <c r="B8" s="64"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="36">
         <v>43990</v>
       </c>
@@ -955,7 +956,7 @@
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
-      <c r="B9" s="64"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="36">
         <v>43992</v>
       </c>
@@ -975,7 +976,7 @@
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
-      <c r="B10" s="64"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="36">
         <v>43994</v>
       </c>
@@ -995,7 +996,7 @@
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
-      <c r="B11" s="64"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="36">
         <v>43996</v>
       </c>
@@ -1015,7 +1016,7 @@
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
-      <c r="B12" s="64"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="36">
         <v>43998</v>
       </c>
@@ -1035,7 +1036,7 @@
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
-      <c r="B13" s="64"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="36">
         <v>44000</v>
       </c>
@@ -1055,7 +1056,7 @@
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
-      <c r="B14" s="64"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="36">
         <v>44002</v>
       </c>
@@ -1075,7 +1076,7 @@
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
-      <c r="B15" s="64"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="36">
         <v>44004</v>
       </c>
@@ -1095,7 +1096,7 @@
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49"/>
-      <c r="B16" s="65"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="36">
         <v>44006</v>
       </c>
@@ -1114,10 +1115,10 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
-        <v>2</v>
-      </c>
-      <c r="B17" s="66" t="s">
+      <c r="A17" s="53">
+        <v>2</v>
+      </c>
+      <c r="B17" s="54" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="37">
@@ -1139,7 +1140,7 @@
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
-      <c r="B18" s="67"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="37">
         <v>43986</v>
       </c>
@@ -1159,7 +1160,7 @@
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
-      <c r="B19" s="67"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="37">
         <v>43987</v>
       </c>
@@ -1179,7 +1180,7 @@
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
-      <c r="B20" s="67"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="37">
         <v>43988</v>
       </c>
@@ -1199,7 +1200,7 @@
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
-      <c r="B21" s="67"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="37">
         <v>43989</v>
       </c>
@@ -1219,7 +1220,7 @@
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
-      <c r="B22" s="67"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="37">
         <v>43990</v>
       </c>
@@ -1239,7 +1240,7 @@
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
-      <c r="B23" s="67"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="37">
         <v>43992</v>
       </c>
@@ -1259,7 +1260,7 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
-      <c r="B24" s="67"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="37">
         <v>43994</v>
       </c>
@@ -1279,7 +1280,7 @@
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
-      <c r="B25" s="67"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="37">
         <v>43996</v>
       </c>
@@ -1299,7 +1300,7 @@
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
-      <c r="B26" s="67"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="37">
         <v>43998</v>
       </c>
@@ -1319,7 +1320,7 @@
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
-      <c r="B27" s="67"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="37">
         <v>44000</v>
       </c>
@@ -1339,7 +1340,7 @@
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
-      <c r="B28" s="67"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37">
         <v>44002</v>
       </c>
@@ -1359,7 +1360,7 @@
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
-      <c r="B29" s="67"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37">
         <v>44004</v>
       </c>
@@ -1379,7 +1380,7 @@
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
-      <c r="B30" s="68"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="37">
         <v>44006</v>
       </c>
@@ -1398,10 +1399,10 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53">
+      <c r="A31" s="48">
         <v>3</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="57" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="36">
@@ -1423,7 +1424,7 @@
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
-      <c r="B32" s="64"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="36">
         <v>43986</v>
       </c>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
-      <c r="B33" s="64"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="36">
         <v>43987</v>
       </c>
@@ -1463,7 +1464,7 @@
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
-      <c r="B34" s="64"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="36">
         <v>43988</v>
       </c>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
-      <c r="B35" s="64"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="36">
         <v>43989</v>
       </c>
@@ -1503,7 +1504,7 @@
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
-      <c r="B36" s="64"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="36">
         <v>43990</v>
       </c>
@@ -1523,7 +1524,7 @@
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
-      <c r="B37" s="64"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="36">
         <v>43992</v>
       </c>
@@ -1543,7 +1544,7 @@
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
-      <c r="B38" s="64"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="36">
         <v>43994</v>
       </c>
@@ -1563,7 +1564,7 @@
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49"/>
-      <c r="B39" s="64"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="36">
         <v>43996</v>
       </c>
@@ -1583,7 +1584,7 @@
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
-      <c r="B40" s="64"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="36">
         <v>43998</v>
       </c>
@@ -1603,7 +1604,7 @@
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49"/>
-      <c r="B41" s="64"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="36">
         <v>44000</v>
       </c>
@@ -1623,7 +1624,7 @@
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
-      <c r="B42" s="64"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="36">
         <v>44002</v>
       </c>
@@ -1643,7 +1644,7 @@
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49"/>
-      <c r="B43" s="64"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="36">
         <v>44004</v>
       </c>
@@ -1663,7 +1664,7 @@
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49"/>
-      <c r="B44" s="65"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="36">
         <v>44006</v>
       </c>
@@ -1682,10 +1683,10 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52">
+      <c r="A45" s="53">
         <v>4</v>
       </c>
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="37">
@@ -1947,7 +1948,7 @@
     </row>
     <row r="58" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49"/>
-      <c r="B58" s="50"/>
+      <c r="B58" s="61"/>
       <c r="C58" s="37">
         <v>44006</v>
       </c>
@@ -1966,10 +1967,10 @@
       <c r="J58" s="22"/>
     </row>
     <row r="59" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53">
+      <c r="A59" s="48">
         <v>5</v>
       </c>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C59" s="36">
@@ -2231,7 +2232,7 @@
     </row>
     <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="49"/>
-      <c r="B72" s="50"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="36">
         <v>44006</v>
       </c>
@@ -2250,10 +2251,10 @@
       <c r="J72" s="6"/>
     </row>
     <row r="73" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="52">
+      <c r="A73" s="53">
         <v>6</v>
       </c>
-      <c r="B73" s="48" t="s">
+      <c r="B73" s="65" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="37">
@@ -2515,7 +2516,7 @@
     </row>
     <row r="86" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="49"/>
-      <c r="B86" s="50"/>
+      <c r="B86" s="61"/>
       <c r="C86" s="37">
         <v>44006</v>
       </c>
@@ -2534,10 +2535,10 @@
       <c r="J86" s="22"/>
     </row>
     <row r="87" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="53">
+      <c r="A87" s="48">
         <v>7</v>
       </c>
-      <c r="B87" s="51" t="s">
+      <c r="B87" s="66" t="s">
         <v>18</v>
       </c>
       <c r="C87" s="36">
@@ -2799,7 +2800,7 @@
     </row>
     <row r="100" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="49"/>
-      <c r="B100" s="50"/>
+      <c r="B100" s="61"/>
       <c r="C100" s="36">
         <v>44006</v>
       </c>
@@ -2818,10 +2819,10 @@
       <c r="J100" s="10"/>
     </row>
     <row r="101" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="52">
+      <c r="A101" s="53">
         <v>8</v>
       </c>
-      <c r="B101" s="48" t="s">
+      <c r="B101" s="65" t="s">
         <v>19</v>
       </c>
       <c r="C101" s="37">
@@ -3083,7 +3084,7 @@
     </row>
     <row r="114" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="49"/>
-      <c r="B114" s="50"/>
+      <c r="B114" s="61"/>
       <c r="C114" s="37">
         <v>44006</v>
       </c>
@@ -3102,10 +3103,10 @@
       <c r="J114" s="22"/>
     </row>
     <row r="115" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="53">
+      <c r="A115" s="48">
         <v>9</v>
       </c>
-      <c r="B115" s="54" t="s">
+      <c r="B115" s="67" t="s">
         <v>20</v>
       </c>
       <c r="C115" s="36">
@@ -3127,7 +3128,7 @@
     </row>
     <row r="116" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="49"/>
-      <c r="B116" s="55"/>
+      <c r="B116" s="68"/>
       <c r="C116" s="36">
         <v>43986</v>
       </c>
@@ -3147,7 +3148,7 @@
     </row>
     <row r="117" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="49"/>
-      <c r="B117" s="55"/>
+      <c r="B117" s="68"/>
       <c r="C117" s="36">
         <v>43987</v>
       </c>
@@ -3167,7 +3168,7 @@
     </row>
     <row r="118" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="49"/>
-      <c r="B118" s="55"/>
+      <c r="B118" s="68"/>
       <c r="C118" s="36">
         <v>43988</v>
       </c>
@@ -3187,7 +3188,7 @@
     </row>
     <row r="119" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="49"/>
-      <c r="B119" s="55"/>
+      <c r="B119" s="68"/>
       <c r="C119" s="36">
         <v>43989</v>
       </c>
@@ -3207,7 +3208,7 @@
     </row>
     <row r="120" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="49"/>
-      <c r="B120" s="55"/>
+      <c r="B120" s="68"/>
       <c r="C120" s="36">
         <v>43990</v>
       </c>
@@ -3227,17 +3228,17 @@
     </row>
     <row r="121" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="49"/>
-      <c r="B121" s="55"/>
+      <c r="B121" s="68"/>
       <c r="C121" s="36">
         <v>43992</v>
       </c>
       <c r="D121" s="36">
         <v>43993</v>
       </c>
-      <c r="E121" s="46">
+      <c r="E121" s="70">
         <v>3</v>
       </c>
-      <c r="F121" s="46">
+      <c r="F121" s="70">
         <v>2</v>
       </c>
       <c r="G121" s="41"/>
@@ -3247,17 +3248,17 @@
     </row>
     <row r="122" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="49"/>
-      <c r="B122" s="55"/>
+      <c r="B122" s="68"/>
       <c r="C122" s="36">
         <v>43994</v>
       </c>
       <c r="D122" s="36">
         <v>43995</v>
       </c>
-      <c r="E122" s="3">
+      <c r="E122" s="44">
         <v>4</v>
       </c>
-      <c r="F122" s="3">
+      <c r="F122" s="44">
         <v>1</v>
       </c>
       <c r="G122" s="38"/>
@@ -3267,17 +3268,17 @@
     </row>
     <row r="123" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="49"/>
-      <c r="B123" s="55"/>
+      <c r="B123" s="68"/>
       <c r="C123" s="36">
         <v>43996</v>
       </c>
       <c r="D123" s="36">
         <v>43997</v>
       </c>
-      <c r="E123" s="3">
+      <c r="E123" s="44">
         <v>4</v>
       </c>
-      <c r="F123" s="3">
+      <c r="F123" s="44">
         <v>2</v>
       </c>
       <c r="G123" s="38"/>
@@ -3287,7 +3288,7 @@
     </row>
     <row r="124" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="49"/>
-      <c r="B124" s="55"/>
+      <c r="B124" s="68"/>
       <c r="C124" s="36">
         <v>43998</v>
       </c>
@@ -3307,7 +3308,7 @@
     </row>
     <row r="125" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="49"/>
-      <c r="B125" s="55"/>
+      <c r="B125" s="68"/>
       <c r="C125" s="36">
         <v>44000</v>
       </c>
@@ -3327,7 +3328,7 @@
     </row>
     <row r="126" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="49"/>
-      <c r="B126" s="55"/>
+      <c r="B126" s="68"/>
       <c r="C126" s="36">
         <v>44002</v>
       </c>
@@ -3347,7 +3348,7 @@
     </row>
     <row r="127" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="49"/>
-      <c r="B127" s="55"/>
+      <c r="B127" s="68"/>
       <c r="C127" s="36">
         <v>44004</v>
       </c>
@@ -3367,7 +3368,7 @@
     </row>
     <row r="128" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="49"/>
-      <c r="B128" s="56"/>
+      <c r="B128" s="69"/>
       <c r="C128" s="36">
         <v>44006</v>
       </c>
@@ -3386,10 +3387,10 @@
       <c r="J128" s="10"/>
     </row>
     <row r="129" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="52">
+      <c r="A129" s="53">
         <v>10</v>
       </c>
-      <c r="B129" s="48" t="s">
+      <c r="B129" s="65" t="s">
         <v>21</v>
       </c>
       <c r="C129" s="37">
@@ -3651,7 +3652,7 @@
     </row>
     <row r="142" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="49"/>
-      <c r="B142" s="50"/>
+      <c r="B142" s="61"/>
       <c r="C142" s="37">
         <v>44006</v>
       </c>
@@ -3670,10 +3671,10 @@
       <c r="J142" s="22"/>
     </row>
     <row r="143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="53">
+      <c r="A143" s="48">
         <v>11</v>
       </c>
-      <c r="B143" s="51" t="s">
+      <c r="B143" s="66" t="s">
         <v>22</v>
       </c>
       <c r="C143" s="36">
@@ -3922,7 +3923,7 @@
     </row>
     <row r="156" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="49"/>
-      <c r="B156" s="50"/>
+      <c r="B156" s="61"/>
       <c r="C156" s="36">
         <v>44006</v>
       </c>
@@ -3940,10 +3941,10 @@
       <c r="I156" s="9"/>
     </row>
     <row r="157" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="52">
+      <c r="A157" s="53">
         <v>12</v>
       </c>
-      <c r="B157" s="48" t="s">
+      <c r="B157" s="65" t="s">
         <v>11</v>
       </c>
       <c r="C157" s="37">
@@ -4205,7 +4206,7 @@
     </row>
     <row r="170" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="49"/>
-      <c r="B170" s="50"/>
+      <c r="B170" s="61"/>
       <c r="C170" s="37">
         <v>44006</v>
       </c>
@@ -4224,10 +4225,10 @@
       <c r="J170" s="22"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="53">
+      <c r="A171" s="48">
         <v>13</v>
       </c>
-      <c r="B171" s="51" t="s">
+      <c r="B171" s="66" t="s">
         <v>10</v>
       </c>
       <c r="C171" s="36">
@@ -4476,7 +4477,7 @@
     </row>
     <row r="184" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="49"/>
-      <c r="B184" s="50"/>
+      <c r="B184" s="61"/>
       <c r="C184" s="36">
         <v>44006</v>
       </c>
@@ -4868,27 +4869,6 @@
     <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="B17:B30"/>
-    <mergeCell ref="A31:A44"/>
-    <mergeCell ref="B31:B44"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B45:B58"/>
-    <mergeCell ref="A45:A58"/>
-    <mergeCell ref="A59:A72"/>
-    <mergeCell ref="A73:A86"/>
-    <mergeCell ref="B59:B72"/>
-    <mergeCell ref="B73:B86"/>
     <mergeCell ref="B157:B170"/>
     <mergeCell ref="B171:B184"/>
     <mergeCell ref="A157:A170"/>
@@ -4903,6 +4883,27 @@
     <mergeCell ref="B143:B156"/>
     <mergeCell ref="A143:A156"/>
     <mergeCell ref="B129:B142"/>
+    <mergeCell ref="B45:B58"/>
+    <mergeCell ref="A45:A58"/>
+    <mergeCell ref="A59:A72"/>
+    <mergeCell ref="A73:A86"/>
+    <mergeCell ref="B59:B72"/>
+    <mergeCell ref="B73:B86"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B17:B30"/>
+    <mergeCell ref="A31:A44"/>
+    <mergeCell ref="B31:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
add bai tap OOP2
</commit_message>
<xml_diff>
--- a/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
+++ b/module1/0.CaseStudy1/Read_me/Check List CaseStudy C0520G1.xlsx
@@ -397,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,10 +498,44 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -510,9 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -526,37 +557,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -791,25 +797,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="62" t="s">
+      <c r="B1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="58" t="s">
@@ -828,13 +834,13 @@
       <c r="G2" s="59"/>
       <c r="H2" s="59"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="61"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48">
-        <v>1</v>
-      </c>
-      <c r="B3" s="50" t="s">
+      <c r="A3" s="54">
+        <v>1</v>
+      </c>
+      <c r="B3" s="64" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="36">
@@ -855,8 +861,8 @@
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="51"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="36">
         <v>43986</v>
       </c>
@@ -875,8 +881,8 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="51"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="36">
         <v>43987</v>
       </c>
@@ -895,8 +901,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="51"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="36">
         <v>43988</v>
       </c>
@@ -915,8 +921,8 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="51"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="36">
         <v>43989</v>
       </c>
@@ -935,8 +941,8 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="51"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="36">
         <v>43990</v>
       </c>
@@ -955,8 +961,8 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="36">
         <v>43992</v>
       </c>
@@ -975,8 +981,8 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="36">
         <v>43994</v>
       </c>
@@ -995,8 +1001,8 @@
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="36">
         <v>43996</v>
       </c>
@@ -1015,8 +1021,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="36">
         <v>43998</v>
       </c>
@@ -1035,8 +1041,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="36">
         <v>44000</v>
       </c>
@@ -1055,8 +1061,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="36">
         <v>44002</v>
       </c>
@@ -1075,8 +1081,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="36">
         <v>44004</v>
       </c>
@@ -1095,8 +1101,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="36">
         <v>44006</v>
       </c>
@@ -1118,7 +1124,7 @@
       <c r="A17" s="53">
         <v>2</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="67" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="37">
@@ -1139,8 +1145,8 @@
       <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="37">
         <v>43986</v>
       </c>
@@ -1159,8 +1165,8 @@
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="37">
         <v>43987</v>
       </c>
@@ -1179,8 +1185,8 @@
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="37">
         <v>43988</v>
       </c>
@@ -1199,8 +1205,8 @@
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="37">
         <v>43989</v>
       </c>
@@ -1219,8 +1225,8 @@
       <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="55"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="37">
         <v>43990</v>
       </c>
@@ -1239,8 +1245,8 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="37">
         <v>43992</v>
       </c>
@@ -1259,8 +1265,8 @@
       <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="55"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="37">
         <v>43994</v>
       </c>
@@ -1279,8 +1285,8 @@
       <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="37">
         <v>43996</v>
       </c>
@@ -1299,8 +1305,8 @@
       <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="37">
         <v>43998</v>
       </c>
@@ -1319,8 +1325,8 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="37">
         <v>44000</v>
       </c>
@@ -1339,8 +1345,8 @@
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="37">
         <v>44002</v>
       </c>
@@ -1359,8 +1365,8 @@
       <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="37">
         <v>44004</v>
       </c>
@@ -1379,8 +1385,8 @@
       <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="69"/>
       <c r="C30" s="37">
         <v>44006</v>
       </c>
@@ -1399,10 +1405,10 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="48">
+      <c r="A31" s="54">
         <v>3</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="70" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="36">
@@ -1423,8 +1429,8 @@
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="51"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="36">
         <v>43986</v>
       </c>
@@ -1443,8 +1449,8 @@
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="51"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="36">
         <v>43987</v>
       </c>
@@ -1463,8 +1469,8 @@
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="36">
         <v>43988</v>
       </c>
@@ -1483,8 +1489,8 @@
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="49"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="36">
         <v>43989</v>
       </c>
@@ -1503,8 +1509,8 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="49"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="50"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="36">
         <v>43990</v>
       </c>
@@ -1523,8 +1529,8 @@
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="36">
         <v>43992</v>
       </c>
@@ -1543,8 +1549,8 @@
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="49"/>
-      <c r="B38" s="51"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="36">
         <v>43994</v>
       </c>
@@ -1563,8 +1569,8 @@
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="49"/>
-      <c r="B39" s="51"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="36">
         <v>43996</v>
       </c>
@@ -1583,8 +1589,8 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="51"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="65"/>
       <c r="C40" s="36">
         <v>43998</v>
       </c>
@@ -1603,8 +1609,8 @@
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="49"/>
-      <c r="B41" s="51"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="65"/>
       <c r="C41" s="36">
         <v>44000</v>
       </c>
@@ -1623,8 +1629,8 @@
       <c r="J41" s="10"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="65"/>
       <c r="C42" s="36">
         <v>44002</v>
       </c>
@@ -1643,8 +1649,8 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="49"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="65"/>
       <c r="C43" s="36">
         <v>44004</v>
       </c>
@@ -1663,8 +1669,8 @@
       <c r="J43" s="10"/>
     </row>
     <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="49"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="50"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="36">
         <v>44006</v>
       </c>
@@ -1686,7 +1692,7 @@
       <c r="A45" s="53">
         <v>4</v>
       </c>
-      <c r="B45" s="65" t="s">
+      <c r="B45" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="37">
@@ -1707,8 +1713,8 @@
       <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="50"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="37">
         <v>43986</v>
       </c>
@@ -1727,8 +1733,8 @@
       <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
-      <c r="B47" s="49"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="50"/>
       <c r="C47" s="37">
         <v>43987</v>
       </c>
@@ -1747,8 +1753,8 @@
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="37">
         <v>43988</v>
       </c>
@@ -1767,8 +1773,8 @@
       <c r="J48" s="20"/>
     </row>
     <row r="49" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="49"/>
-      <c r="B49" s="49"/>
+      <c r="A49" s="50"/>
+      <c r="B49" s="50"/>
       <c r="C49" s="37">
         <v>43989</v>
       </c>
@@ -1787,8 +1793,8 @@
       <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49"/>
-      <c r="B50" s="49"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="37">
         <v>43990</v>
       </c>
@@ -1807,8 +1813,8 @@
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
-      <c r="B51" s="49"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="37">
         <v>43992</v>
       </c>
@@ -1827,8 +1833,8 @@
       <c r="J51" s="22"/>
     </row>
     <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49"/>
-      <c r="B52" s="49"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="37">
         <v>43994</v>
       </c>
@@ -1847,8 +1853,8 @@
       <c r="J52" s="22"/>
     </row>
     <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
-      <c r="B53" s="49"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="37">
         <v>43996</v>
       </c>
@@ -1867,8 +1873,8 @@
       <c r="J53" s="22"/>
     </row>
     <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
-      <c r="B54" s="49"/>
+      <c r="A54" s="50"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="37">
         <v>43998</v>
       </c>
@@ -1887,8 +1893,8 @@
       <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="49"/>
-      <c r="B55" s="49"/>
+      <c r="A55" s="50"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="37">
         <v>44000</v>
       </c>
@@ -1907,8 +1913,8 @@
       <c r="J55" s="22"/>
     </row>
     <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
-      <c r="B56" s="49"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="50"/>
       <c r="C56" s="37">
         <v>44002</v>
       </c>
@@ -1927,8 +1933,8 @@
       <c r="J56" s="22"/>
     </row>
     <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="49"/>
-      <c r="B57" s="49"/>
+      <c r="A57" s="50"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="37">
         <v>44004</v>
       </c>
@@ -1947,8 +1953,8 @@
       <c r="J57" s="22"/>
     </row>
     <row r="58" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="49"/>
-      <c r="B58" s="61"/>
+      <c r="A58" s="50"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="37">
         <v>44006</v>
       </c>
@@ -1967,10 +1973,10 @@
       <c r="J58" s="22"/>
     </row>
     <row r="59" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="48">
+      <c r="A59" s="54">
         <v>5</v>
       </c>
-      <c r="B59" s="66" t="s">
+      <c r="B59" s="52" t="s">
         <v>16</v>
       </c>
       <c r="C59" s="36">
@@ -1991,8 +1997,8 @@
       <c r="J59" s="6"/>
     </row>
     <row r="60" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="49"/>
-      <c r="B60" s="49"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="50"/>
       <c r="C60" s="36">
         <v>43986</v>
       </c>
@@ -2011,8 +2017,8 @@
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="49"/>
-      <c r="B61" s="49"/>
+      <c r="A61" s="50"/>
+      <c r="B61" s="50"/>
       <c r="C61" s="36">
         <v>43987</v>
       </c>
@@ -2031,8 +2037,8 @@
       <c r="J61" s="6"/>
     </row>
     <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="49"/>
-      <c r="B62" s="49"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="50"/>
       <c r="C62" s="36">
         <v>43988</v>
       </c>
@@ -2051,8 +2057,8 @@
       <c r="J62" s="6"/>
     </row>
     <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="49"/>
-      <c r="B63" s="49"/>
+      <c r="A63" s="50"/>
+      <c r="B63" s="50"/>
       <c r="C63" s="36">
         <v>43989</v>
       </c>
@@ -2071,8 +2077,8 @@
       <c r="J63" s="6"/>
     </row>
     <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="49"/>
-      <c r="B64" s="49"/>
+      <c r="A64" s="50"/>
+      <c r="B64" s="50"/>
       <c r="C64" s="36">
         <v>43990</v>
       </c>
@@ -2091,8 +2097,8 @@
       <c r="J64" s="6"/>
     </row>
     <row r="65" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="49"/>
-      <c r="B65" s="49"/>
+      <c r="A65" s="50"/>
+      <c r="B65" s="50"/>
       <c r="C65" s="36">
         <v>43992</v>
       </c>
@@ -2111,8 +2117,8 @@
       <c r="J65" s="6"/>
     </row>
     <row r="66" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="49"/>
-      <c r="B66" s="49"/>
+      <c r="A66" s="50"/>
+      <c r="B66" s="50"/>
       <c r="C66" s="36">
         <v>43994</v>
       </c>
@@ -2131,8 +2137,8 @@
       <c r="J66" s="6"/>
     </row>
     <row r="67" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="49"/>
-      <c r="B67" s="49"/>
+      <c r="A67" s="50"/>
+      <c r="B67" s="50"/>
       <c r="C67" s="36">
         <v>43996</v>
       </c>
@@ -2151,8 +2157,8 @@
       <c r="J67" s="6"/>
     </row>
     <row r="68" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="49"/>
-      <c r="B68" s="49"/>
+      <c r="A68" s="50"/>
+      <c r="B68" s="50"/>
       <c r="C68" s="36">
         <v>43998</v>
       </c>
@@ -2171,8 +2177,8 @@
       <c r="J68" s="6"/>
     </row>
     <row r="69" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="49"/>
-      <c r="B69" s="49"/>
+      <c r="A69" s="50"/>
+      <c r="B69" s="50"/>
       <c r="C69" s="36">
         <v>44000</v>
       </c>
@@ -2191,8 +2197,8 @@
       <c r="J69" s="6"/>
     </row>
     <row r="70" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="49"/>
-      <c r="B70" s="49"/>
+      <c r="A70" s="50"/>
+      <c r="B70" s="50"/>
       <c r="C70" s="36">
         <v>44002</v>
       </c>
@@ -2211,8 +2217,8 @@
       <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="49"/>
-      <c r="B71" s="49"/>
+      <c r="A71" s="50"/>
+      <c r="B71" s="50"/>
       <c r="C71" s="36">
         <v>44004</v>
       </c>
@@ -2231,8 +2237,8 @@
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="49"/>
-      <c r="B72" s="61"/>
+      <c r="A72" s="50"/>
+      <c r="B72" s="51"/>
       <c r="C72" s="36">
         <v>44006</v>
       </c>
@@ -2254,7 +2260,7 @@
       <c r="A73" s="53">
         <v>6</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B73" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C73" s="37">
@@ -2275,8 +2281,8 @@
       <c r="J73" s="20"/>
     </row>
     <row r="74" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="49"/>
-      <c r="B74" s="49"/>
+      <c r="A74" s="50"/>
+      <c r="B74" s="50"/>
       <c r="C74" s="37">
         <v>43986</v>
       </c>
@@ -2295,8 +2301,8 @@
       <c r="J74" s="20"/>
     </row>
     <row r="75" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="49"/>
-      <c r="B75" s="49"/>
+      <c r="A75" s="50"/>
+      <c r="B75" s="50"/>
       <c r="C75" s="37">
         <v>43987</v>
       </c>
@@ -2315,8 +2321,8 @@
       <c r="J75" s="20"/>
     </row>
     <row r="76" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="49"/>
-      <c r="B76" s="49"/>
+      <c r="A76" s="50"/>
+      <c r="B76" s="50"/>
       <c r="C76" s="37">
         <v>43988</v>
       </c>
@@ -2335,8 +2341,8 @@
       <c r="J76" s="20"/>
     </row>
     <row r="77" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="49"/>
-      <c r="B77" s="49"/>
+      <c r="A77" s="50"/>
+      <c r="B77" s="50"/>
       <c r="C77" s="37">
         <v>43989</v>
       </c>
@@ -2355,8 +2361,8 @@
       <c r="J77" s="20"/>
     </row>
     <row r="78" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="49"/>
-      <c r="B78" s="49"/>
+      <c r="A78" s="50"/>
+      <c r="B78" s="50"/>
       <c r="C78" s="37">
         <v>43990</v>
       </c>
@@ -2375,8 +2381,8 @@
       <c r="J78" s="20"/>
     </row>
     <row r="79" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="49"/>
-      <c r="B79" s="49"/>
+      <c r="A79" s="50"/>
+      <c r="B79" s="50"/>
       <c r="C79" s="37">
         <v>43992</v>
       </c>
@@ -2395,8 +2401,8 @@
       <c r="J79" s="22"/>
     </row>
     <row r="80" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="49"/>
-      <c r="B80" s="49"/>
+      <c r="A80" s="50"/>
+      <c r="B80" s="50"/>
       <c r="C80" s="37">
         <v>43994</v>
       </c>
@@ -2415,8 +2421,8 @@
       <c r="J80" s="22"/>
     </row>
     <row r="81" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="49"/>
-      <c r="B81" s="49"/>
+      <c r="A81" s="50"/>
+      <c r="B81" s="50"/>
       <c r="C81" s="37">
         <v>43996</v>
       </c>
@@ -2435,8 +2441,8 @@
       <c r="J81" s="22"/>
     </row>
     <row r="82" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="49"/>
-      <c r="B82" s="49"/>
+      <c r="A82" s="50"/>
+      <c r="B82" s="50"/>
       <c r="C82" s="37">
         <v>43998</v>
       </c>
@@ -2455,8 +2461,8 @@
       <c r="J82" s="22"/>
     </row>
     <row r="83" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="49"/>
-      <c r="B83" s="49"/>
+      <c r="A83" s="50"/>
+      <c r="B83" s="50"/>
       <c r="C83" s="37">
         <v>44000</v>
       </c>
@@ -2475,8 +2481,8 @@
       <c r="J83" s="22"/>
     </row>
     <row r="84" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="49"/>
-      <c r="B84" s="49"/>
+      <c r="A84" s="50"/>
+      <c r="B84" s="50"/>
       <c r="C84" s="37">
         <v>44002</v>
       </c>
@@ -2495,8 +2501,8 @@
       <c r="J84" s="22"/>
     </row>
     <row r="85" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="49"/>
-      <c r="B85" s="49"/>
+      <c r="A85" s="50"/>
+      <c r="B85" s="50"/>
       <c r="C85" s="37">
         <v>44004</v>
       </c>
@@ -2515,8 +2521,8 @@
       <c r="J85" s="22"/>
     </row>
     <row r="86" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="49"/>
-      <c r="B86" s="61"/>
+      <c r="A86" s="50"/>
+      <c r="B86" s="51"/>
       <c r="C86" s="37">
         <v>44006</v>
       </c>
@@ -2535,10 +2541,10 @@
       <c r="J86" s="22"/>
     </row>
     <row r="87" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="48">
+      <c r="A87" s="54">
         <v>7</v>
       </c>
-      <c r="B87" s="66" t="s">
+      <c r="B87" s="52" t="s">
         <v>18</v>
       </c>
       <c r="C87" s="36">
@@ -2559,8 +2565,8 @@
       <c r="J87" s="6"/>
     </row>
     <row r="88" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="49"/>
-      <c r="B88" s="49"/>
+      <c r="A88" s="50"/>
+      <c r="B88" s="50"/>
       <c r="C88" s="36">
         <v>43986</v>
       </c>
@@ -2579,8 +2585,8 @@
       <c r="J88" s="6"/>
     </row>
     <row r="89" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="49"/>
-      <c r="B89" s="49"/>
+      <c r="A89" s="50"/>
+      <c r="B89" s="50"/>
       <c r="C89" s="36">
         <v>43987</v>
       </c>
@@ -2599,8 +2605,8 @@
       <c r="J89" s="6"/>
     </row>
     <row r="90" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="49"/>
-      <c r="B90" s="49"/>
+      <c r="A90" s="50"/>
+      <c r="B90" s="50"/>
       <c r="C90" s="36">
         <v>43988</v>
       </c>
@@ -2619,8 +2625,8 @@
       <c r="J90" s="6"/>
     </row>
     <row r="91" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="49"/>
-      <c r="B91" s="49"/>
+      <c r="A91" s="50"/>
+      <c r="B91" s="50"/>
       <c r="C91" s="36">
         <v>43989</v>
       </c>
@@ -2639,8 +2645,8 @@
       <c r="J91" s="6"/>
     </row>
     <row r="92" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="49"/>
-      <c r="B92" s="49"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="50"/>
       <c r="C92" s="36">
         <v>43990</v>
       </c>
@@ -2659,8 +2665,8 @@
       <c r="J92" s="6"/>
     </row>
     <row r="93" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="49"/>
-      <c r="B93" s="49"/>
+      <c r="A93" s="50"/>
+      <c r="B93" s="50"/>
       <c r="C93" s="36">
         <v>43992</v>
       </c>
@@ -2679,8 +2685,8 @@
       <c r="J93" s="10"/>
     </row>
     <row r="94" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="49"/>
-      <c r="B94" s="49"/>
+      <c r="A94" s="50"/>
+      <c r="B94" s="50"/>
       <c r="C94" s="36">
         <v>43994</v>
       </c>
@@ -2699,8 +2705,8 @@
       <c r="J94" s="10"/>
     </row>
     <row r="95" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="49"/>
-      <c r="B95" s="49"/>
+      <c r="A95" s="50"/>
+      <c r="B95" s="50"/>
       <c r="C95" s="36">
         <v>43996</v>
       </c>
@@ -2719,8 +2725,8 @@
       <c r="J95" s="10"/>
     </row>
     <row r="96" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="49"/>
-      <c r="B96" s="49"/>
+      <c r="A96" s="50"/>
+      <c r="B96" s="50"/>
       <c r="C96" s="36">
         <v>43998</v>
       </c>
@@ -2739,8 +2745,8 @@
       <c r="J96" s="10"/>
     </row>
     <row r="97" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="49"/>
-      <c r="B97" s="49"/>
+      <c r="A97" s="50"/>
+      <c r="B97" s="50"/>
       <c r="C97" s="36">
         <v>44000</v>
       </c>
@@ -2759,8 +2765,8 @@
       <c r="J97" s="10"/>
     </row>
     <row r="98" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="49"/>
-      <c r="B98" s="49"/>
+      <c r="A98" s="50"/>
+      <c r="B98" s="50"/>
       <c r="C98" s="36">
         <v>44002</v>
       </c>
@@ -2779,8 +2785,8 @@
       <c r="J98" s="10"/>
     </row>
     <row r="99" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="49"/>
-      <c r="B99" s="49"/>
+      <c r="A99" s="50"/>
+      <c r="B99" s="50"/>
       <c r="C99" s="36">
         <v>44004</v>
       </c>
@@ -2799,8 +2805,8 @@
       <c r="J99" s="10"/>
     </row>
     <row r="100" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="49"/>
-      <c r="B100" s="61"/>
+      <c r="A100" s="50"/>
+      <c r="B100" s="51"/>
       <c r="C100" s="36">
         <v>44006</v>
       </c>
@@ -2822,7 +2828,7 @@
       <c r="A101" s="53">
         <v>8</v>
       </c>
-      <c r="B101" s="65" t="s">
+      <c r="B101" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C101" s="37">
@@ -2843,8 +2849,8 @@
       <c r="J101" s="20"/>
     </row>
     <row r="102" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="49"/>
-      <c r="B102" s="49"/>
+      <c r="A102" s="50"/>
+      <c r="B102" s="50"/>
       <c r="C102" s="37">
         <v>43986</v>
       </c>
@@ -2863,8 +2869,8 @@
       <c r="J102" s="20"/>
     </row>
     <row r="103" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="49"/>
-      <c r="B103" s="49"/>
+      <c r="A103" s="50"/>
+      <c r="B103" s="50"/>
       <c r="C103" s="37">
         <v>43987</v>
       </c>
@@ -2883,8 +2889,8 @@
       <c r="J103" s="20"/>
     </row>
     <row r="104" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="49"/>
-      <c r="B104" s="49"/>
+      <c r="A104" s="50"/>
+      <c r="B104" s="50"/>
       <c r="C104" s="37">
         <v>43988</v>
       </c>
@@ -2903,8 +2909,8 @@
       <c r="J104" s="20"/>
     </row>
     <row r="105" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="49"/>
-      <c r="B105" s="49"/>
+      <c r="A105" s="50"/>
+      <c r="B105" s="50"/>
       <c r="C105" s="37">
         <v>43989</v>
       </c>
@@ -2923,8 +2929,8 @@
       <c r="J105" s="20"/>
     </row>
     <row r="106" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="49"/>
-      <c r="B106" s="49"/>
+      <c r="A106" s="50"/>
+      <c r="B106" s="50"/>
       <c r="C106" s="37">
         <v>43990</v>
       </c>
@@ -2943,8 +2949,8 @@
       <c r="J106" s="20"/>
     </row>
     <row r="107" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="49"/>
-      <c r="B107" s="49"/>
+      <c r="A107" s="50"/>
+      <c r="B107" s="50"/>
       <c r="C107" s="37">
         <v>43992</v>
       </c>
@@ -2963,8 +2969,8 @@
       <c r="J107" s="22"/>
     </row>
     <row r="108" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="49"/>
-      <c r="B108" s="49"/>
+      <c r="A108" s="50"/>
+      <c r="B108" s="50"/>
       <c r="C108" s="37">
         <v>43994</v>
       </c>
@@ -2983,8 +2989,8 @@
       <c r="J108" s="22"/>
     </row>
     <row r="109" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="49"/>
-      <c r="B109" s="49"/>
+      <c r="A109" s="50"/>
+      <c r="B109" s="50"/>
       <c r="C109" s="37">
         <v>43996</v>
       </c>
@@ -3003,8 +3009,8 @@
       <c r="J109" s="22"/>
     </row>
     <row r="110" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="49"/>
-      <c r="B110" s="49"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="50"/>
       <c r="C110" s="37">
         <v>43998</v>
       </c>
@@ -3023,8 +3029,8 @@
       <c r="J110" s="22"/>
     </row>
     <row r="111" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="49"/>
-      <c r="B111" s="49"/>
+      <c r="A111" s="50"/>
+      <c r="B111" s="50"/>
       <c r="C111" s="37">
         <v>44000</v>
       </c>
@@ -3043,8 +3049,8 @@
       <c r="J111" s="22"/>
     </row>
     <row r="112" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="49"/>
-      <c r="B112" s="49"/>
+      <c r="A112" s="50"/>
+      <c r="B112" s="50"/>
       <c r="C112" s="37">
         <v>44002</v>
       </c>
@@ -3063,8 +3069,8 @@
       <c r="J112" s="22"/>
     </row>
     <row r="113" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="49"/>
-      <c r="B113" s="49"/>
+      <c r="A113" s="50"/>
+      <c r="B113" s="50"/>
       <c r="C113" s="37">
         <v>44004</v>
       </c>
@@ -3083,8 +3089,8 @@
       <c r="J113" s="22"/>
     </row>
     <row r="114" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="49"/>
-      <c r="B114" s="61"/>
+      <c r="A114" s="50"/>
+      <c r="B114" s="51"/>
       <c r="C114" s="37">
         <v>44006</v>
       </c>
@@ -3103,10 +3109,10 @@
       <c r="J114" s="22"/>
     </row>
     <row r="115" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="48">
+      <c r="A115" s="54">
         <v>9</v>
       </c>
-      <c r="B115" s="67" t="s">
+      <c r="B115" s="55" t="s">
         <v>20</v>
       </c>
       <c r="C115" s="36">
@@ -3127,8 +3133,8 @@
       <c r="J115" s="6"/>
     </row>
     <row r="116" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="49"/>
-      <c r="B116" s="68"/>
+      <c r="A116" s="50"/>
+      <c r="B116" s="56"/>
       <c r="C116" s="36">
         <v>43986</v>
       </c>
@@ -3147,8 +3153,8 @@
       <c r="J116" s="6"/>
     </row>
     <row r="117" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="49"/>
-      <c r="B117" s="68"/>
+      <c r="A117" s="50"/>
+      <c r="B117" s="56"/>
       <c r="C117" s="36">
         <v>43987</v>
       </c>
@@ -3167,8 +3173,8 @@
       <c r="J117" s="6"/>
     </row>
     <row r="118" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="49"/>
-      <c r="B118" s="68"/>
+      <c r="A118" s="50"/>
+      <c r="B118" s="56"/>
       <c r="C118" s="36">
         <v>43988</v>
       </c>
@@ -3187,8 +3193,8 @@
       <c r="J118" s="6"/>
     </row>
     <row r="119" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="49"/>
-      <c r="B119" s="68"/>
+      <c r="A119" s="50"/>
+      <c r="B119" s="56"/>
       <c r="C119" s="36">
         <v>43989</v>
       </c>
@@ -3207,8 +3213,8 @@
       <c r="J119" s="6"/>
     </row>
     <row r="120" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="49"/>
-      <c r="B120" s="68"/>
+      <c r="A120" s="50"/>
+      <c r="B120" s="56"/>
       <c r="C120" s="36">
         <v>43990</v>
       </c>
@@ -3227,18 +3233,18 @@
       <c r="J120" s="6"/>
     </row>
     <row r="121" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="49"/>
-      <c r="B121" s="68"/>
+      <c r="A121" s="50"/>
+      <c r="B121" s="56"/>
       <c r="C121" s="36">
         <v>43992</v>
       </c>
       <c r="D121" s="36">
         <v>43993</v>
       </c>
-      <c r="E121" s="70">
+      <c r="E121" s="48">
         <v>3</v>
       </c>
-      <c r="F121" s="70">
+      <c r="F121" s="48">
         <v>2</v>
       </c>
       <c r="G121" s="41"/>
@@ -3247,8 +3253,8 @@
       <c r="J121" s="10"/>
     </row>
     <row r="122" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="49"/>
-      <c r="B122" s="68"/>
+      <c r="A122" s="50"/>
+      <c r="B122" s="56"/>
       <c r="C122" s="36">
         <v>43994</v>
       </c>
@@ -3267,8 +3273,8 @@
       <c r="J122" s="10"/>
     </row>
     <row r="123" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="49"/>
-      <c r="B123" s="68"/>
+      <c r="A123" s="50"/>
+      <c r="B123" s="56"/>
       <c r="C123" s="36">
         <v>43996</v>
       </c>
@@ -3287,18 +3293,18 @@
       <c r="J123" s="10"/>
     </row>
     <row r="124" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="49"/>
-      <c r="B124" s="68"/>
+      <c r="A124" s="50"/>
+      <c r="B124" s="56"/>
       <c r="C124" s="36">
         <v>43998</v>
       </c>
       <c r="D124" s="36">
         <v>43999</v>
       </c>
-      <c r="E124" s="3">
+      <c r="E124" s="44">
         <v>5</v>
       </c>
-      <c r="F124" s="11" t="s">
+      <c r="F124" s="71" t="s">
         <v>7</v>
       </c>
       <c r="G124" s="40"/>
@@ -3307,18 +3313,18 @@
       <c r="J124" s="10"/>
     </row>
     <row r="125" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="49"/>
-      <c r="B125" s="68"/>
+      <c r="A125" s="50"/>
+      <c r="B125" s="56"/>
       <c r="C125" s="36">
         <v>44000</v>
       </c>
       <c r="D125" s="36">
         <v>44001</v>
       </c>
-      <c r="E125" s="3">
+      <c r="E125" s="44">
         <v>5</v>
       </c>
-      <c r="F125" s="13" t="s">
+      <c r="F125" s="72" t="s">
         <v>8</v>
       </c>
       <c r="G125" s="38"/>
@@ -3327,8 +3333,8 @@
       <c r="J125" s="10"/>
     </row>
     <row r="126" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="49"/>
-      <c r="B126" s="68"/>
+      <c r="A126" s="50"/>
+      <c r="B126" s="56"/>
       <c r="C126" s="36">
         <v>44002</v>
       </c>
@@ -3347,8 +3353,8 @@
       <c r="J126" s="10"/>
     </row>
     <row r="127" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="49"/>
-      <c r="B127" s="68"/>
+      <c r="A127" s="50"/>
+      <c r="B127" s="56"/>
       <c r="C127" s="36">
         <v>44004</v>
       </c>
@@ -3367,8 +3373,8 @@
       <c r="J127" s="10"/>
     </row>
     <row r="128" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="49"/>
-      <c r="B128" s="69"/>
+      <c r="A128" s="50"/>
+      <c r="B128" s="57"/>
       <c r="C128" s="36">
         <v>44006</v>
       </c>
@@ -3390,7 +3396,7 @@
       <c r="A129" s="53">
         <v>10</v>
       </c>
-      <c r="B129" s="65" t="s">
+      <c r="B129" s="49" t="s">
         <v>21</v>
       </c>
       <c r="C129" s="37">
@@ -3411,8 +3417,8 @@
       <c r="J129" s="20"/>
     </row>
     <row r="130" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="49"/>
-      <c r="B130" s="49"/>
+      <c r="A130" s="50"/>
+      <c r="B130" s="50"/>
       <c r="C130" s="37">
         <v>43986</v>
       </c>
@@ -3431,8 +3437,8 @@
       <c r="J130" s="20"/>
     </row>
     <row r="131" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="49"/>
-      <c r="B131" s="49"/>
+      <c r="A131" s="50"/>
+      <c r="B131" s="50"/>
       <c r="C131" s="37">
         <v>43987</v>
       </c>
@@ -3451,8 +3457,8 @@
       <c r="J131" s="20"/>
     </row>
     <row r="132" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="49"/>
-      <c r="B132" s="49"/>
+      <c r="A132" s="50"/>
+      <c r="B132" s="50"/>
       <c r="C132" s="37">
         <v>43988</v>
       </c>
@@ -3471,8 +3477,8 @@
       <c r="J132" s="20"/>
     </row>
     <row r="133" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="49"/>
-      <c r="B133" s="49"/>
+      <c r="A133" s="50"/>
+      <c r="B133" s="50"/>
       <c r="C133" s="37">
         <v>43989</v>
       </c>
@@ -3491,8 +3497,8 @@
       <c r="J133" s="20"/>
     </row>
     <row r="134" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="49"/>
-      <c r="B134" s="49"/>
+      <c r="A134" s="50"/>
+      <c r="B134" s="50"/>
       <c r="C134" s="37">
         <v>43990</v>
       </c>
@@ -3511,8 +3517,8 @@
       <c r="J134" s="20"/>
     </row>
     <row r="135" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="49"/>
-      <c r="B135" s="49"/>
+      <c r="A135" s="50"/>
+      <c r="B135" s="50"/>
       <c r="C135" s="37">
         <v>43992</v>
       </c>
@@ -3531,8 +3537,8 @@
       <c r="J135" s="22"/>
     </row>
     <row r="136" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="49"/>
-      <c r="B136" s="49"/>
+      <c r="A136" s="50"/>
+      <c r="B136" s="50"/>
       <c r="C136" s="37">
         <v>43994</v>
       </c>
@@ -3551,8 +3557,8 @@
       <c r="J136" s="22"/>
     </row>
     <row r="137" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="49"/>
-      <c r="B137" s="49"/>
+      <c r="A137" s="50"/>
+      <c r="B137" s="50"/>
       <c r="C137" s="37">
         <v>43996</v>
       </c>
@@ -3571,8 +3577,8 @@
       <c r="J137" s="22"/>
     </row>
     <row r="138" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="49"/>
-      <c r="B138" s="49"/>
+      <c r="A138" s="50"/>
+      <c r="B138" s="50"/>
       <c r="C138" s="37">
         <v>43998</v>
       </c>
@@ -3591,8 +3597,8 @@
       <c r="J138" s="22"/>
     </row>
     <row r="139" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="49"/>
-      <c r="B139" s="49"/>
+      <c r="A139" s="50"/>
+      <c r="B139" s="50"/>
       <c r="C139" s="37">
         <v>44000</v>
       </c>
@@ -3611,8 +3617,8 @@
       <c r="J139" s="22"/>
     </row>
     <row r="140" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="49"/>
-      <c r="B140" s="49"/>
+      <c r="A140" s="50"/>
+      <c r="B140" s="50"/>
       <c r="C140" s="37">
         <v>44002</v>
       </c>
@@ -3631,8 +3637,8 @@
       <c r="J140" s="22"/>
     </row>
     <row r="141" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="49"/>
-      <c r="B141" s="49"/>
+      <c r="A141" s="50"/>
+      <c r="B141" s="50"/>
       <c r="C141" s="37">
         <v>44004</v>
       </c>
@@ -3651,8 +3657,8 @@
       <c r="J141" s="22"/>
     </row>
     <row r="142" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="49"/>
-      <c r="B142" s="61"/>
+      <c r="A142" s="50"/>
+      <c r="B142" s="51"/>
       <c r="C142" s="37">
         <v>44006</v>
       </c>
@@ -3671,10 +3677,10 @@
       <c r="J142" s="22"/>
     </row>
     <row r="143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="48">
+      <c r="A143" s="54">
         <v>11</v>
       </c>
-      <c r="B143" s="66" t="s">
+      <c r="B143" s="52" t="s">
         <v>22</v>
       </c>
       <c r="C143" s="36">
@@ -3694,8 +3700,8 @@
       <c r="I143" s="5"/>
     </row>
     <row r="144" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="49"/>
-      <c r="B144" s="49"/>
+      <c r="A144" s="50"/>
+      <c r="B144" s="50"/>
       <c r="C144" s="36">
         <v>43986</v>
       </c>
@@ -3713,8 +3719,8 @@
       <c r="I144" s="7"/>
     </row>
     <row r="145" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="49"/>
-      <c r="B145" s="49"/>
+      <c r="A145" s="50"/>
+      <c r="B145" s="50"/>
       <c r="C145" s="36">
         <v>43987</v>
       </c>
@@ -3732,8 +3738,8 @@
       <c r="I145" s="7"/>
     </row>
     <row r="146" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="49"/>
-      <c r="B146" s="49"/>
+      <c r="A146" s="50"/>
+      <c r="B146" s="50"/>
       <c r="C146" s="36">
         <v>43988</v>
       </c>
@@ -3751,8 +3757,8 @@
       <c r="I146" s="7"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="49"/>
-      <c r="B147" s="49"/>
+      <c r="A147" s="50"/>
+      <c r="B147" s="50"/>
       <c r="C147" s="36">
         <v>43989</v>
       </c>
@@ -3770,8 +3776,8 @@
       <c r="I147" s="7"/>
     </row>
     <row r="148" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="49"/>
-      <c r="B148" s="49"/>
+      <c r="A148" s="50"/>
+      <c r="B148" s="50"/>
       <c r="C148" s="36">
         <v>43990</v>
       </c>
@@ -3789,8 +3795,8 @@
       <c r="I148" s="7"/>
     </row>
     <row r="149" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="49"/>
-      <c r="B149" s="49"/>
+      <c r="A149" s="50"/>
+      <c r="B149" s="50"/>
       <c r="C149" s="36">
         <v>43992</v>
       </c>
@@ -3808,8 +3814,8 @@
       <c r="I149" s="7"/>
     </row>
     <row r="150" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="49"/>
-      <c r="B150" s="49"/>
+      <c r="A150" s="50"/>
+      <c r="B150" s="50"/>
       <c r="C150" s="36">
         <v>43994</v>
       </c>
@@ -3827,8 +3833,8 @@
       <c r="I150" s="7"/>
     </row>
     <row r="151" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="49"/>
-      <c r="B151" s="49"/>
+      <c r="A151" s="50"/>
+      <c r="B151" s="50"/>
       <c r="C151" s="36">
         <v>43996</v>
       </c>
@@ -3846,8 +3852,8 @@
       <c r="I151" s="7"/>
     </row>
     <row r="152" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="49"/>
-      <c r="B152" s="49"/>
+      <c r="A152" s="50"/>
+      <c r="B152" s="50"/>
       <c r="C152" s="36">
         <v>43998</v>
       </c>
@@ -3865,8 +3871,8 @@
       <c r="I152" s="12"/>
     </row>
     <row r="153" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="49"/>
-      <c r="B153" s="49"/>
+      <c r="A153" s="50"/>
+      <c r="B153" s="50"/>
       <c r="C153" s="36">
         <v>44000</v>
       </c>
@@ -3884,8 +3890,8 @@
       <c r="I153" s="12"/>
     </row>
     <row r="154" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="49"/>
-      <c r="B154" s="49"/>
+      <c r="A154" s="50"/>
+      <c r="B154" s="50"/>
       <c r="C154" s="36">
         <v>44002</v>
       </c>
@@ -3903,8 +3909,8 @@
       <c r="I154" s="12"/>
     </row>
     <row r="155" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="49"/>
-      <c r="B155" s="49"/>
+      <c r="A155" s="50"/>
+      <c r="B155" s="50"/>
       <c r="C155" s="36">
         <v>44004</v>
       </c>
@@ -3922,8 +3928,8 @@
       <c r="I155" s="12"/>
     </row>
     <row r="156" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="49"/>
-      <c r="B156" s="61"/>
+      <c r="A156" s="50"/>
+      <c r="B156" s="51"/>
       <c r="C156" s="36">
         <v>44006</v>
       </c>
@@ -3944,7 +3950,7 @@
       <c r="A157" s="53">
         <v>12</v>
       </c>
-      <c r="B157" s="65" t="s">
+      <c r="B157" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C157" s="37">
@@ -3965,8 +3971,8 @@
       <c r="J157" s="20"/>
     </row>
     <row r="158" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="49"/>
-      <c r="B158" s="49"/>
+      <c r="A158" s="50"/>
+      <c r="B158" s="50"/>
       <c r="C158" s="37">
         <v>43986</v>
       </c>
@@ -3985,8 +3991,8 @@
       <c r="J158" s="20"/>
     </row>
     <row r="159" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="49"/>
-      <c r="B159" s="49"/>
+      <c r="A159" s="50"/>
+      <c r="B159" s="50"/>
       <c r="C159" s="37">
         <v>43987</v>
       </c>
@@ -4005,8 +4011,8 @@
       <c r="J159" s="20"/>
     </row>
     <row r="160" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="49"/>
-      <c r="B160" s="49"/>
+      <c r="A160" s="50"/>
+      <c r="B160" s="50"/>
       <c r="C160" s="37">
         <v>43988</v>
       </c>
@@ -4025,8 +4031,8 @@
       <c r="J160" s="20"/>
     </row>
     <row r="161" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="49"/>
-      <c r="B161" s="49"/>
+      <c r="A161" s="50"/>
+      <c r="B161" s="50"/>
       <c r="C161" s="37">
         <v>43989</v>
       </c>
@@ -4045,8 +4051,8 @@
       <c r="J161" s="20"/>
     </row>
     <row r="162" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="49"/>
-      <c r="B162" s="49"/>
+      <c r="A162" s="50"/>
+      <c r="B162" s="50"/>
       <c r="C162" s="37">
         <v>43990</v>
       </c>
@@ -4065,8 +4071,8 @@
       <c r="J162" s="20"/>
     </row>
     <row r="163" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="49"/>
-      <c r="B163" s="49"/>
+      <c r="A163" s="50"/>
+      <c r="B163" s="50"/>
       <c r="C163" s="37">
         <v>43992</v>
       </c>
@@ -4085,8 +4091,8 @@
       <c r="J163" s="22"/>
     </row>
     <row r="164" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="49"/>
-      <c r="B164" s="49"/>
+      <c r="A164" s="50"/>
+      <c r="B164" s="50"/>
       <c r="C164" s="37">
         <v>43994</v>
       </c>
@@ -4105,8 +4111,8 @@
       <c r="J164" s="22"/>
     </row>
     <row r="165" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="49"/>
-      <c r="B165" s="49"/>
+      <c r="A165" s="50"/>
+      <c r="B165" s="50"/>
       <c r="C165" s="37">
         <v>43996</v>
       </c>
@@ -4125,8 +4131,8 @@
       <c r="J165" s="22"/>
     </row>
     <row r="166" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="49"/>
-      <c r="B166" s="49"/>
+      <c r="A166" s="50"/>
+      <c r="B166" s="50"/>
       <c r="C166" s="37">
         <v>43998</v>
       </c>
@@ -4145,8 +4151,8 @@
       <c r="J166" s="22"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="49"/>
-      <c r="B167" s="49"/>
+      <c r="A167" s="50"/>
+      <c r="B167" s="50"/>
       <c r="C167" s="37">
         <v>44000</v>
       </c>
@@ -4165,8 +4171,8 @@
       <c r="J167" s="22"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="49"/>
-      <c r="B168" s="49"/>
+      <c r="A168" s="50"/>
+      <c r="B168" s="50"/>
       <c r="C168" s="37">
         <v>44002</v>
       </c>
@@ -4185,8 +4191,8 @@
       <c r="J168" s="22"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="49"/>
-      <c r="B169" s="49"/>
+      <c r="A169" s="50"/>
+      <c r="B169" s="50"/>
       <c r="C169" s="37">
         <v>44004</v>
       </c>
@@ -4205,8 +4211,8 @@
       <c r="J169" s="22"/>
     </row>
     <row r="170" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="49"/>
-      <c r="B170" s="61"/>
+      <c r="A170" s="50"/>
+      <c r="B170" s="51"/>
       <c r="C170" s="37">
         <v>44006</v>
       </c>
@@ -4225,10 +4231,10 @@
       <c r="J170" s="22"/>
     </row>
     <row r="171" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="48">
+      <c r="A171" s="54">
         <v>13</v>
       </c>
-      <c r="B171" s="66" t="s">
+      <c r="B171" s="52" t="s">
         <v>10</v>
       </c>
       <c r="C171" s="36">
@@ -4248,8 +4254,8 @@
       <c r="I171" s="5"/>
     </row>
     <row r="172" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="49"/>
-      <c r="B172" s="49"/>
+      <c r="A172" s="50"/>
+      <c r="B172" s="50"/>
       <c r="C172" s="36">
         <v>43986</v>
       </c>
@@ -4267,8 +4273,8 @@
       <c r="I172" s="7"/>
     </row>
     <row r="173" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="49"/>
-      <c r="B173" s="49"/>
+      <c r="A173" s="50"/>
+      <c r="B173" s="50"/>
       <c r="C173" s="36">
         <v>43987</v>
       </c>
@@ -4286,8 +4292,8 @@
       <c r="I173" s="7"/>
     </row>
     <row r="174" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="49"/>
-      <c r="B174" s="49"/>
+      <c r="A174" s="50"/>
+      <c r="B174" s="50"/>
       <c r="C174" s="36">
         <v>43988</v>
       </c>
@@ -4305,8 +4311,8 @@
       <c r="I174" s="7"/>
     </row>
     <row r="175" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="49"/>
-      <c r="B175" s="49"/>
+      <c r="A175" s="50"/>
+      <c r="B175" s="50"/>
       <c r="C175" s="36">
         <v>43989</v>
       </c>
@@ -4324,8 +4330,8 @@
       <c r="I175" s="7"/>
     </row>
     <row r="176" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="49"/>
-      <c r="B176" s="49"/>
+      <c r="A176" s="50"/>
+      <c r="B176" s="50"/>
       <c r="C176" s="36">
         <v>43990</v>
       </c>
@@ -4343,8 +4349,8 @@
       <c r="I176" s="7"/>
     </row>
     <row r="177" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="49"/>
-      <c r="B177" s="49"/>
+      <c r="A177" s="50"/>
+      <c r="B177" s="50"/>
       <c r="C177" s="36">
         <v>43992</v>
       </c>
@@ -4362,8 +4368,8 @@
       <c r="I177" s="7"/>
     </row>
     <row r="178" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="49"/>
-      <c r="B178" s="49"/>
+      <c r="A178" s="50"/>
+      <c r="B178" s="50"/>
       <c r="C178" s="36">
         <v>43994</v>
       </c>
@@ -4381,8 +4387,8 @@
       <c r="I178" s="7"/>
     </row>
     <row r="179" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="49"/>
-      <c r="B179" s="49"/>
+      <c r="A179" s="50"/>
+      <c r="B179" s="50"/>
       <c r="C179" s="36">
         <v>43996</v>
       </c>
@@ -4400,8 +4406,8 @@
       <c r="I179" s="9"/>
     </row>
     <row r="180" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="49"/>
-      <c r="B180" s="49"/>
+      <c r="A180" s="50"/>
+      <c r="B180" s="50"/>
       <c r="C180" s="36">
         <v>43998</v>
       </c>
@@ -4419,8 +4425,8 @@
       <c r="I180" s="12"/>
     </row>
     <row r="181" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="49"/>
-      <c r="B181" s="49"/>
+      <c r="A181" s="50"/>
+      <c r="B181" s="50"/>
       <c r="C181" s="36">
         <v>44000</v>
       </c>
@@ -4438,8 +4444,8 @@
       <c r="I181" s="12"/>
     </row>
     <row r="182" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="49"/>
-      <c r="B182" s="49"/>
+      <c r="A182" s="50"/>
+      <c r="B182" s="50"/>
       <c r="C182" s="36">
         <v>44002</v>
       </c>
@@ -4457,8 +4463,8 @@
       <c r="I182" s="12"/>
     </row>
     <row r="183" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="49"/>
-      <c r="B183" s="49"/>
+      <c r="A183" s="50"/>
+      <c r="B183" s="50"/>
       <c r="C183" s="36">
         <v>44004</v>
       </c>
@@ -4476,8 +4482,8 @@
       <c r="I183" s="12"/>
     </row>
     <row r="184" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="49"/>
-      <c r="B184" s="61"/>
+      <c r="A184" s="50"/>
+      <c r="B184" s="51"/>
       <c r="C184" s="36">
         <v>44006</v>
       </c>
@@ -4869,6 +4875,27 @@
     <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B17:B30"/>
+    <mergeCell ref="A31:A44"/>
+    <mergeCell ref="B31:B44"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B45:B58"/>
+    <mergeCell ref="A45:A58"/>
+    <mergeCell ref="A59:A72"/>
+    <mergeCell ref="A73:A86"/>
+    <mergeCell ref="B59:B72"/>
+    <mergeCell ref="B73:B86"/>
     <mergeCell ref="B157:B170"/>
     <mergeCell ref="B171:B184"/>
     <mergeCell ref="A157:A170"/>
@@ -4883,27 +4910,6 @@
     <mergeCell ref="B143:B156"/>
     <mergeCell ref="A143:A156"/>
     <mergeCell ref="B129:B142"/>
-    <mergeCell ref="B45:B58"/>
-    <mergeCell ref="A45:A58"/>
-    <mergeCell ref="A59:A72"/>
-    <mergeCell ref="A73:A86"/>
-    <mergeCell ref="B59:B72"/>
-    <mergeCell ref="B73:B86"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="B17:B30"/>
-    <mergeCell ref="A31:A44"/>
-    <mergeCell ref="B31:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>